<commit_message>
Criteria_Ranking added in excel reader
</commit_message>
<xml_diff>
--- a/Criteria Ranking.xlsx
+++ b/Criteria Ranking.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33EB939-F641-4CD8-A66A-0FDA8AD91073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F435461-AB11-41E9-980E-C5B96A54F63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="4" state="hidden" r:id="rId2"/>
-    <sheet name="DATA Percentage" sheetId="6" state="hidden" r:id="rId3"/>
-    <sheet name="DATA Ranking" sheetId="7" state="hidden" r:id="rId4"/>
+    <sheet name="DATA Percentage" sheetId="6" r:id="rId3"/>
+    <sheet name="DATA Ranking" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'DATA Percentage'!$B$1:$D$20</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="261">
   <si>
     <t xml:space="preserve">Safety </t>
   </si>
@@ -1226,17 +1226,68 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1260,57 +1311,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2037,8 +2037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4261850-8DA1-46EB-8872-E313C5418792}">
   <dimension ref="B1:AK208"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="102" zoomScaleNormal="87" zoomScaleSheetLayoutView="64" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView showGridLines="0" topLeftCell="B88" zoomScale="102" zoomScaleNormal="87" zoomScaleSheetLayoutView="64" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89:T95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,31 +2061,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
       <c r="Y1" s="18"/>
       <c r="Z1" s="8"/>
       <c r="AA1" s="8"/>
@@ -2101,29 +2101,29 @@
       <c r="AK1" s="8"/>
     </row>
     <row r="2" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
       <c r="Y2" s="18"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
@@ -2139,10 +2139,10 @@
       <c r="AK2" s="8"/>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2179,31 +2179,31 @@
       <c r="AK3" s="8"/>
     </row>
     <row r="4" spans="2:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
       <c r="Y4" s="18"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
@@ -2219,31 +2219,31 @@
       <c r="AK4" s="8"/>
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="42"/>
       <c r="Y5" s="18"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
@@ -2259,29 +2259,29 @@
       <c r="AK5" s="8"/>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
+      <c r="X6" s="42"/>
       <c r="Y6" s="18"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
@@ -2297,29 +2297,29 @@
       <c r="AK6" s="8"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
       <c r="Y7" s="18"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
@@ -2335,31 +2335,31 @@
       <c r="AK7" s="8"/>
     </row>
     <row r="8" spans="2:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
       <c r="Y8" s="18"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
@@ -2375,31 +2375,31 @@
       <c r="AK8" s="8"/>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="42"/>
+      <c r="X9" s="42"/>
       <c r="Y9" s="18"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
@@ -2415,29 +2415,29 @@
       <c r="AK9" s="8"/>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="42"/>
+      <c r="X10" s="42"/>
       <c r="Y10" s="18"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8"/>
@@ -2453,31 +2453,31 @@
       <c r="AK10" s="8"/>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
       <c r="Y11" s="18"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
@@ -2493,29 +2493,29 @@
       <c r="AK11" s="8"/>
     </row>
     <row r="12" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
       <c r="Y12" s="18"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
@@ -2531,31 +2531,31 @@
       <c r="AK12" s="8"/>
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="33"/>
-      <c r="U13" s="33"/>
-      <c r="V13" s="33"/>
-      <c r="W13" s="33"/>
-      <c r="X13" s="34"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="51"/>
       <c r="Y13" s="18"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
@@ -2571,29 +2571,29 @@
       <c r="AK13" s="8"/>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="34"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="51"/>
       <c r="Y14" s="18"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
@@ -2650,32 +2650,32 @@
       <c r="B16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="23" t="s">
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="31" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="23" t="s">
+      <c r="L16" s="48"/>
+      <c r="M16" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="31" t="s">
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -2797,12 +2797,12 @@
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="8"/>
-      <c r="T18" s="25" t="s">
+      <c r="T18" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="18"/>
       <c r="Z18" s="8"/>
@@ -3468,11 +3468,11 @@
         <v>26</v>
       </c>
       <c r="R26" s="8"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="V26" s="42"/>
+      <c r="W26" s="42"/>
       <c r="X26" s="8"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="8"/>
@@ -3556,11 +3556,11 @@
         <v>26</v>
       </c>
       <c r="R27" s="8"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="18"/>
       <c r="Z27" s="8"/>
@@ -3643,11 +3643,11 @@
         <v>26</v>
       </c>
       <c r="R28" s="8"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="42"/>
+      <c r="V28" s="42"/>
+      <c r="W28" s="42"/>
       <c r="X28" s="8"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="8"/>
@@ -4124,27 +4124,27 @@
       <c r="AK33" s="8"/>
     </row>
     <row r="34" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="38"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="38"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
       <c r="U34" s="8"/>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
@@ -4168,25 +4168,25 @@
       <c r="AK34" s="8"/>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="40"/>
+      <c r="R35" s="40"/>
+      <c r="S35" s="40"/>
+      <c r="T35" s="40"/>
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
@@ -4248,10 +4248,10 @@
       <c r="AK36" s="8"/>
     </row>
     <row r="37" spans="2:37" ht="21" x14ac:dyDescent="0.4">
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="24"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
@@ -4339,37 +4339,37 @@
       <c r="AK38" s="8"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="39" t="s">
+      <c r="G39" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
       <c r="O39" s="16"/>
       <c r="P39" s="8"/>
-      <c r="Q39" s="37" t="s">
+      <c r="Q39" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="R39" s="37"/>
-      <c r="S39" s="37"/>
-      <c r="T39" s="37"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="34"/>
       <c r="U39" s="8"/>
-      <c r="V39" s="36" t="s">
+      <c r="V39" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
+      <c r="W39" s="35"/>
+      <c r="X39" s="35"/>
       <c r="Y39" s="18"/>
       <c r="Z39" s="8"/>
       <c r="AA39" s="8" t="s">
@@ -4389,37 +4389,37 @@
       <c r="AK39" s="8"/>
     </row>
     <row r="40" spans="2:37" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
       <c r="O40" s="13"/>
       <c r="P40" s="8"/>
-      <c r="Q40" s="35" t="s">
+      <c r="Q40" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
       <c r="U40" s="13"/>
-      <c r="V40" s="35" t="s">
+      <c r="V40" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
       <c r="Y40" s="18"/>
       <c r="Z40" s="8"/>
       <c r="AA40" s="8" t="s">
@@ -4479,37 +4479,37 @@
       <c r="AK41" s="8"/>
     </row>
     <row r="42" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
       <c r="O42" s="1"/>
       <c r="P42" s="8"/>
-      <c r="Q42" s="36" t="s">
+      <c r="Q42" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="R42" s="36"/>
-      <c r="S42" s="36"/>
-      <c r="T42" s="36"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
       <c r="U42" s="8"/>
-      <c r="V42" s="36" t="s">
+      <c r="V42" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
       <c r="Y42" s="18"/>
       <c r="Z42" s="8"/>
       <c r="AA42" s="8" t="s">
@@ -4527,37 +4527,37 @@
       <c r="AK42" s="8"/>
     </row>
     <row r="43" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="35" t="s">
+      <c r="G43" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
       <c r="O43" s="15"/>
       <c r="P43" s="8"/>
-      <c r="Q43" s="43" t="s">
+      <c r="Q43" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="R43" s="44"/>
-      <c r="S43" s="44"/>
-      <c r="T43" s="44"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
       <c r="U43" s="8"/>
-      <c r="V43" s="43" t="s">
+      <c r="V43" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="W43" s="44"/>
-      <c r="X43" s="44"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
       <c r="Y43" s="18"/>
       <c r="Z43" s="8"/>
       <c r="AA43" s="8" t="s">
@@ -4577,29 +4577,29 @@
       <c r="AK43" s="8"/>
     </row>
     <row r="44" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
       <c r="O44" s="15"/>
       <c r="P44" s="8"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="44"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
       <c r="U44" s="8"/>
-      <c r="V44" s="44"/>
-      <c r="W44" s="44"/>
-      <c r="X44" s="44"/>
+      <c r="V44" s="37"/>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
       <c r="Y44" s="18"/>
       <c r="Z44" s="8"/>
       <c r="AA44" s="8" t="s">
@@ -4619,29 +4619,29 @@
       <c r="AK44" s="8"/>
     </row>
     <row r="45" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
       <c r="O45" s="15"/>
       <c r="P45" s="8"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
       <c r="U45" s="8"/>
-      <c r="V45" s="44"/>
-      <c r="W45" s="44"/>
-      <c r="X45" s="44"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
       <c r="Y45" s="18"/>
       <c r="Z45" s="8"/>
       <c r="AA45" s="8" t="s">
@@ -4659,29 +4659,29 @@
       <c r="AK45" s="8"/>
     </row>
     <row r="46" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
       <c r="O46" s="15"/>
       <c r="P46" s="8"/>
-      <c r="Q46" s="44"/>
-      <c r="R46" s="44"/>
-      <c r="S46" s="44"/>
-      <c r="T46" s="44"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
       <c r="U46" s="8"/>
-      <c r="V46" s="44"/>
-      <c r="W46" s="44"/>
-      <c r="X46" s="44"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
       <c r="Y46" s="18"/>
       <c r="Z46" s="8"/>
       <c r="AA46" s="8" t="s">
@@ -4701,29 +4701,29 @@
       <c r="AK46" s="8"/>
     </row>
     <row r="47" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
-      <c r="N47" s="35"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
       <c r="O47" s="15"/>
       <c r="P47" s="8"/>
-      <c r="Q47" s="44"/>
-      <c r="R47" s="44"/>
-      <c r="S47" s="44"/>
-      <c r="T47" s="44"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
       <c r="U47" s="8"/>
-      <c r="V47" s="44"/>
-      <c r="W47" s="44"/>
-      <c r="X47" s="44"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
       <c r="Y47" s="18"/>
       <c r="Z47" s="8"/>
       <c r="AA47" s="8" t="s">
@@ -4743,29 +4743,29 @@
       <c r="AK47" s="8"/>
     </row>
     <row r="48" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="35"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
       <c r="O48" s="15"/>
       <c r="P48" s="8"/>
-      <c r="Q48" s="44"/>
-      <c r="R48" s="44"/>
-      <c r="S48" s="44"/>
-      <c r="T48" s="44"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
       <c r="U48" s="8"/>
-      <c r="V48" s="44"/>
-      <c r="W48" s="44"/>
-      <c r="X48" s="44"/>
+      <c r="V48" s="37"/>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
       <c r="Y48" s="18"/>
       <c r="Z48" s="8"/>
       <c r="AA48" s="8" t="s">
@@ -4785,29 +4785,29 @@
       <c r="AK48" s="8"/>
     </row>
     <row r="49" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
       <c r="O49" s="15"/>
       <c r="P49" s="8"/>
-      <c r="Q49" s="44"/>
-      <c r="R49" s="44"/>
-      <c r="S49" s="44"/>
-      <c r="T49" s="44"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
       <c r="U49" s="8"/>
-      <c r="V49" s="44"/>
-      <c r="W49" s="44"/>
-      <c r="X49" s="44"/>
+      <c r="V49" s="37"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
       <c r="Y49" s="18"/>
       <c r="Z49" s="8"/>
       <c r="AA49" s="8" t="s">
@@ -4827,29 +4827,29 @@
       <c r="AK49" s="8"/>
     </row>
     <row r="50" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
-      <c r="N50" s="35"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="32"/>
+      <c r="N50" s="32"/>
       <c r="O50" s="15"/>
       <c r="P50" s="8"/>
-      <c r="Q50" s="44"/>
-      <c r="R50" s="44"/>
-      <c r="S50" s="44"/>
-      <c r="T50" s="44"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
       <c r="U50" s="8"/>
-      <c r="V50" s="44"/>
-      <c r="W50" s="44"/>
-      <c r="X50" s="44"/>
+      <c r="V50" s="37"/>
+      <c r="W50" s="37"/>
+      <c r="X50" s="37"/>
       <c r="Y50" s="18"/>
       <c r="Z50" s="8"/>
       <c r="AA50" s="8" t="s">
@@ -4869,29 +4869,29 @@
       <c r="AK50" s="8"/>
     </row>
     <row r="51" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="35"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
       <c r="O51" s="15"/>
       <c r="P51" s="8"/>
-      <c r="Q51" s="44"/>
-      <c r="R51" s="44"/>
-      <c r="S51" s="44"/>
-      <c r="T51" s="44"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
       <c r="U51" s="8"/>
-      <c r="V51" s="44"/>
-      <c r="W51" s="44"/>
-      <c r="X51" s="44"/>
+      <c r="V51" s="37"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="37"/>
       <c r="Y51" s="18"/>
       <c r="Z51" s="8"/>
       <c r="AA51" s="8" t="s">
@@ -4911,25 +4911,25 @@
       <c r="AK51" s="8"/>
     </row>
     <row r="52" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="35"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="35"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
       <c r="O52" s="15"/>
       <c r="P52" s="8"/>
-      <c r="Q52" s="44"/>
-      <c r="R52" s="44"/>
-      <c r="S52" s="44"/>
-      <c r="T52" s="44"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
+      <c r="S52" s="37"/>
+      <c r="T52" s="37"/>
       <c r="U52" s="8"/>
       <c r="V52" s="8"/>
       <c r="W52" s="8"/>
@@ -4953,19 +4953,19 @@
       <c r="AK52" s="8"/>
     </row>
     <row r="53" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="8"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="32"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32"/>
       <c r="O53" s="8"/>
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
@@ -4995,19 +4995,19 @@
       <c r="AK53" s="8"/>
     </row>
     <row r="54" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
-      <c r="N54" s="35"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="32"/>
+      <c r="N54" s="32"/>
       <c r="O54" s="8"/>
       <c r="P54" s="8"/>
       <c r="Q54" s="8"/>
@@ -5077,37 +5077,37 @@
       <c r="AK55" s="8"/>
     </row>
     <row r="56" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
       <c r="F56" s="8"/>
-      <c r="G56" s="36" t="s">
+      <c r="G56" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="36"/>
-      <c r="M56" s="36"/>
-      <c r="N56" s="36"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
       <c r="O56" s="8"/>
-      <c r="P56" s="36" t="s">
+      <c r="P56" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Q56" s="36"/>
-      <c r="R56" s="36"/>
-      <c r="S56" s="36"/>
-      <c r="T56" s="36"/>
+      <c r="Q56" s="35"/>
+      <c r="R56" s="35"/>
+      <c r="S56" s="35"/>
+      <c r="T56" s="35"/>
       <c r="U56" s="8"/>
-      <c r="V56" s="36" t="s">
+      <c r="V56" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="W56" s="36"/>
-      <c r="X56" s="36"/>
+      <c r="W56" s="35"/>
+      <c r="X56" s="35"/>
       <c r="Y56" s="18"/>
       <c r="Z56" s="8"/>
       <c r="AA56" s="8" t="s">
@@ -5127,37 +5127,37 @@
       <c r="AK56" s="8"/>
     </row>
     <row r="57" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="35" t="s">
+      <c r="G57" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="32"/>
+      <c r="N57" s="32"/>
       <c r="O57" s="8"/>
-      <c r="P57" s="26" t="s">
+      <c r="P57" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="Q57" s="26"/>
-      <c r="R57" s="26"/>
-      <c r="S57" s="26"/>
-      <c r="T57" s="26"/>
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
+      <c r="S57" s="38"/>
+      <c r="T57" s="38"/>
       <c r="U57" s="8"/>
-      <c r="V57" s="35" t="s">
+      <c r="V57" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="W57" s="35"/>
-      <c r="X57" s="35"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="32"/>
       <c r="Y57" s="18"/>
       <c r="Z57" s="8"/>
       <c r="AA57" s="8" t="s">
@@ -5177,29 +5177,29 @@
       <c r="AK57" s="8"/>
     </row>
     <row r="58" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
       <c r="O58" s="8"/>
-      <c r="P58" s="26"/>
-      <c r="Q58" s="26"/>
-      <c r="R58" s="26"/>
-      <c r="S58" s="26"/>
-      <c r="T58" s="26"/>
+      <c r="P58" s="38"/>
+      <c r="Q58" s="38"/>
+      <c r="R58" s="38"/>
+      <c r="S58" s="38"/>
+      <c r="T58" s="38"/>
       <c r="U58" s="8"/>
-      <c r="V58" s="35"/>
-      <c r="W58" s="35"/>
-      <c r="X58" s="35"/>
+      <c r="V58" s="32"/>
+      <c r="W58" s="32"/>
+      <c r="X58" s="32"/>
       <c r="Y58" s="18"/>
       <c r="Z58" s="8"/>
       <c r="AA58" s="8" t="s">
@@ -5219,29 +5219,29 @@
       <c r="AK58" s="8"/>
     </row>
     <row r="59" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
       <c r="F59" s="8"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
       <c r="O59" s="8"/>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26"/>
-      <c r="T59" s="26"/>
+      <c r="P59" s="38"/>
+      <c r="Q59" s="38"/>
+      <c r="R59" s="38"/>
+      <c r="S59" s="38"/>
+      <c r="T59" s="38"/>
       <c r="U59" s="8"/>
-      <c r="V59" s="35"/>
-      <c r="W59" s="35"/>
-      <c r="X59" s="35"/>
+      <c r="V59" s="32"/>
+      <c r="W59" s="32"/>
+      <c r="X59" s="32"/>
       <c r="Y59" s="18"/>
       <c r="Z59" s="8"/>
       <c r="AA59" s="8" t="s">
@@ -5261,29 +5261,29 @@
       <c r="AK59" s="8"/>
     </row>
     <row r="60" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B60" s="35"/>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
       <c r="F60" s="8"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
       <c r="O60" s="8"/>
-      <c r="P60" s="26"/>
-      <c r="Q60" s="26"/>
-      <c r="R60" s="26"/>
-      <c r="S60" s="26"/>
-      <c r="T60" s="26"/>
+      <c r="P60" s="38"/>
+      <c r="Q60" s="38"/>
+      <c r="R60" s="38"/>
+      <c r="S60" s="38"/>
+      <c r="T60" s="38"/>
       <c r="U60" s="8"/>
-      <c r="V60" s="35"/>
-      <c r="W60" s="35"/>
-      <c r="X60" s="35"/>
+      <c r="V60" s="32"/>
+      <c r="W60" s="32"/>
+      <c r="X60" s="32"/>
       <c r="Y60" s="18"/>
       <c r="Z60" s="8"/>
       <c r="AA60" s="8" t="s">
@@ -5303,29 +5303,29 @@
       <c r="AK60" s="8"/>
     </row>
     <row r="61" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
       <c r="O61" s="8"/>
-      <c r="P61" s="26"/>
-      <c r="Q61" s="26"/>
-      <c r="R61" s="26"/>
-      <c r="S61" s="26"/>
-      <c r="T61" s="26"/>
+      <c r="P61" s="38"/>
+      <c r="Q61" s="38"/>
+      <c r="R61" s="38"/>
+      <c r="S61" s="38"/>
+      <c r="T61" s="38"/>
       <c r="U61" s="8"/>
-      <c r="V61" s="35"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="35"/>
+      <c r="V61" s="32"/>
+      <c r="W61" s="32"/>
+      <c r="X61" s="32"/>
       <c r="Y61" s="18"/>
       <c r="Z61" s="8"/>
       <c r="AA61" s="8" t="s">
@@ -5345,29 +5345,29 @@
       <c r="AK61" s="8"/>
     </row>
     <row r="62" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
       <c r="F62" s="8"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="32"/>
+      <c r="L62" s="32"/>
+      <c r="M62" s="32"/>
+      <c r="N62" s="32"/>
       <c r="O62" s="8"/>
-      <c r="P62" s="26"/>
-      <c r="Q62" s="26"/>
-      <c r="R62" s="26"/>
-      <c r="S62" s="26"/>
-      <c r="T62" s="26"/>
+      <c r="P62" s="38"/>
+      <c r="Q62" s="38"/>
+      <c r="R62" s="38"/>
+      <c r="S62" s="38"/>
+      <c r="T62" s="38"/>
       <c r="U62" s="8"/>
-      <c r="V62" s="35"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
+      <c r="V62" s="32"/>
+      <c r="W62" s="32"/>
+      <c r="X62" s="32"/>
       <c r="Y62" s="18"/>
       <c r="Z62" s="8"/>
       <c r="AA62" s="8" t="s">
@@ -5387,29 +5387,29 @@
       <c r="AK62" s="8"/>
     </row>
     <row r="63" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
       <c r="O63" s="8"/>
-      <c r="P63" s="26"/>
-      <c r="Q63" s="26"/>
-      <c r="R63" s="26"/>
-      <c r="S63" s="26"/>
-      <c r="T63" s="26"/>
+      <c r="P63" s="38"/>
+      <c r="Q63" s="38"/>
+      <c r="R63" s="38"/>
+      <c r="S63" s="38"/>
+      <c r="T63" s="38"/>
       <c r="U63" s="8"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
+      <c r="V63" s="32"/>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
       <c r="Y63" s="18"/>
       <c r="Z63" s="8"/>
       <c r="AA63" s="8" t="s">
@@ -5429,29 +5429,29 @@
       <c r="AK63" s="8"/>
     </row>
     <row r="64" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="35"/>
-      <c r="K64" s="35"/>
-      <c r="L64" s="35"/>
-      <c r="M64" s="35"/>
-      <c r="N64" s="35"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
       <c r="O64" s="8"/>
-      <c r="P64" s="26"/>
-      <c r="Q64" s="26"/>
-      <c r="R64" s="26"/>
-      <c r="S64" s="26"/>
-      <c r="T64" s="26"/>
+      <c r="P64" s="38"/>
+      <c r="Q64" s="38"/>
+      <c r="R64" s="38"/>
+      <c r="S64" s="38"/>
+      <c r="T64" s="38"/>
       <c r="U64" s="8"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
+      <c r="V64" s="32"/>
+      <c r="W64" s="32"/>
+      <c r="X64" s="32"/>
       <c r="Y64" s="18"/>
       <c r="Z64" s="8"/>
       <c r="AA64" s="8" t="s">
@@ -5471,29 +5471,29 @@
       <c r="AK64" s="8"/>
     </row>
     <row r="65" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
       <c r="F65" s="8"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
       <c r="O65" s="8"/>
-      <c r="P65" s="26"/>
-      <c r="Q65" s="26"/>
-      <c r="R65" s="26"/>
-      <c r="S65" s="26"/>
-      <c r="T65" s="26"/>
+      <c r="P65" s="38"/>
+      <c r="Q65" s="38"/>
+      <c r="R65" s="38"/>
+      <c r="S65" s="38"/>
+      <c r="T65" s="38"/>
       <c r="U65" s="8"/>
-      <c r="V65" s="35"/>
-      <c r="W65" s="35"/>
-      <c r="X65" s="35"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="32"/>
+      <c r="X65" s="32"/>
       <c r="Y65" s="18"/>
       <c r="Z65" s="8"/>
       <c r="AA65" s="8" t="s">
@@ -5513,29 +5513,29 @@
       <c r="AK65" s="8"/>
     </row>
     <row r="66" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-      <c r="M66" s="35"/>
-      <c r="N66" s="35"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="32"/>
+      <c r="K66" s="32"/>
+      <c r="L66" s="32"/>
+      <c r="M66" s="32"/>
+      <c r="N66" s="32"/>
       <c r="O66" s="8"/>
-      <c r="P66" s="26"/>
-      <c r="Q66" s="26"/>
-      <c r="R66" s="26"/>
-      <c r="S66" s="26"/>
-      <c r="T66" s="26"/>
+      <c r="P66" s="38"/>
+      <c r="Q66" s="38"/>
+      <c r="R66" s="38"/>
+      <c r="S66" s="38"/>
+      <c r="T66" s="38"/>
       <c r="U66" s="8"/>
-      <c r="V66" s="35"/>
-      <c r="W66" s="35"/>
-      <c r="X66" s="35"/>
+      <c r="V66" s="32"/>
+      <c r="W66" s="32"/>
+      <c r="X66" s="32"/>
       <c r="Y66" s="18"/>
       <c r="Z66" s="8"/>
       <c r="AA66" s="8" t="s">
@@ -5553,29 +5553,29 @@
       <c r="AK66" s="8"/>
     </row>
     <row r="67" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
-      <c r="K67" s="35"/>
-      <c r="L67" s="35"/>
-      <c r="M67" s="35"/>
-      <c r="N67" s="35"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="32"/>
+      <c r="L67" s="32"/>
+      <c r="M67" s="32"/>
+      <c r="N67" s="32"/>
       <c r="O67" s="8"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="26"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
+      <c r="P67" s="38"/>
+      <c r="Q67" s="38"/>
+      <c r="R67" s="38"/>
+      <c r="S67" s="38"/>
+      <c r="T67" s="38"/>
       <c r="U67" s="8"/>
-      <c r="V67" s="35"/>
-      <c r="W67" s="35"/>
-      <c r="X67" s="35"/>
+      <c r="V67" s="32"/>
+      <c r="W67" s="32"/>
+      <c r="X67" s="32"/>
       <c r="Y67" s="18"/>
       <c r="Z67" s="8"/>
       <c r="AA67" s="8" t="s">
@@ -5635,31 +5635,31 @@
       <c r="AK68" s="8"/>
     </row>
     <row r="69" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="36" t="s">
+      <c r="G69" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-      <c r="J69" s="36"/>
-      <c r="K69" s="36"/>
-      <c r="L69" s="36"/>
-      <c r="M69" s="36"/>
-      <c r="N69" s="36"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="L69" s="35"/>
+      <c r="M69" s="35"/>
+      <c r="N69" s="35"/>
       <c r="O69" s="8"/>
-      <c r="P69" s="36" t="s">
+      <c r="P69" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="Q69" s="36"/>
-      <c r="R69" s="36"/>
-      <c r="S69" s="36"/>
-      <c r="T69" s="36"/>
+      <c r="Q69" s="35"/>
+      <c r="R69" s="35"/>
+      <c r="S69" s="35"/>
+      <c r="T69" s="35"/>
       <c r="U69" s="8"/>
       <c r="V69" s="13"/>
       <c r="W69" s="13"/>
@@ -5681,31 +5681,31 @@
       <c r="AK69" s="8"/>
     </row>
     <row r="70" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="35" t="s">
+      <c r="G70" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H70" s="35"/>
-      <c r="I70" s="35"/>
-      <c r="J70" s="35"/>
-      <c r="K70" s="35"/>
-      <c r="L70" s="35"/>
-      <c r="M70" s="35"/>
-      <c r="N70" s="35"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="32"/>
+      <c r="L70" s="32"/>
+      <c r="M70" s="32"/>
+      <c r="N70" s="32"/>
       <c r="O70" s="8"/>
-      <c r="P70" s="35" t="s">
+      <c r="P70" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="Q70" s="35"/>
-      <c r="R70" s="35"/>
-      <c r="S70" s="35"/>
-      <c r="T70" s="35"/>
+      <c r="Q70" s="32"/>
+      <c r="R70" s="32"/>
+      <c r="S70" s="32"/>
+      <c r="T70" s="32"/>
       <c r="U70" s="8"/>
       <c r="V70" s="13"/>
       <c r="W70" s="13"/>
@@ -5727,25 +5727,25 @@
       <c r="AK70" s="8"/>
     </row>
     <row r="71" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="35"/>
-      <c r="L71" s="35"/>
-      <c r="M71" s="35"/>
-      <c r="N71" s="35"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="32"/>
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="32"/>
       <c r="O71" s="8"/>
-      <c r="P71" s="35"/>
-      <c r="Q71" s="35"/>
-      <c r="R71" s="35"/>
-      <c r="S71" s="35"/>
-      <c r="T71" s="35"/>
+      <c r="P71" s="32"/>
+      <c r="Q71" s="32"/>
+      <c r="R71" s="32"/>
+      <c r="S71" s="32"/>
+      <c r="T71" s="32"/>
       <c r="U71" s="8"/>
       <c r="V71" s="13"/>
       <c r="W71" s="13"/>
@@ -5767,25 +5767,25 @@
       <c r="AK71" s="8"/>
     </row>
     <row r="72" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
-      <c r="K72" s="35"/>
-      <c r="L72" s="35"/>
-      <c r="M72" s="35"/>
-      <c r="N72" s="35"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="32"/>
+      <c r="L72" s="32"/>
+      <c r="M72" s="32"/>
+      <c r="N72" s="32"/>
       <c r="O72" s="8"/>
-      <c r="P72" s="35"/>
-      <c r="Q72" s="35"/>
-      <c r="R72" s="35"/>
-      <c r="S72" s="35"/>
-      <c r="T72" s="35"/>
+      <c r="P72" s="32"/>
+      <c r="Q72" s="32"/>
+      <c r="R72" s="32"/>
+      <c r="S72" s="32"/>
+      <c r="T72" s="32"/>
       <c r="U72" s="8"/>
       <c r="V72" s="13"/>
       <c r="W72" s="13"/>
@@ -5809,25 +5809,25 @@
       <c r="AK72" s="8"/>
     </row>
     <row r="73" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
       <c r="F73" s="8"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="35"/>
-      <c r="I73" s="35"/>
-      <c r="J73" s="35"/>
-      <c r="K73" s="35"/>
-      <c r="L73" s="35"/>
-      <c r="M73" s="35"/>
-      <c r="N73" s="35"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="32"/>
+      <c r="J73" s="32"/>
+      <c r="K73" s="32"/>
+      <c r="L73" s="32"/>
+      <c r="M73" s="32"/>
+      <c r="N73" s="32"/>
       <c r="O73" s="8"/>
-      <c r="P73" s="35"/>
-      <c r="Q73" s="35"/>
-      <c r="R73" s="35"/>
-      <c r="S73" s="35"/>
-      <c r="T73" s="35"/>
+      <c r="P73" s="32"/>
+      <c r="Q73" s="32"/>
+      <c r="R73" s="32"/>
+      <c r="S73" s="32"/>
+      <c r="T73" s="32"/>
       <c r="U73" s="8"/>
       <c r="V73" s="8"/>
       <c r="W73" s="8"/>
@@ -5851,25 +5851,25 @@
       <c r="AK73" s="8"/>
     </row>
     <row r="74" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
       <c r="F74" s="8"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="35"/>
-      <c r="I74" s="35"/>
-      <c r="J74" s="35"/>
-      <c r="K74" s="35"/>
-      <c r="L74" s="35"/>
-      <c r="M74" s="35"/>
-      <c r="N74" s="35"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="32"/>
+      <c r="K74" s="32"/>
+      <c r="L74" s="32"/>
+      <c r="M74" s="32"/>
+      <c r="N74" s="32"/>
       <c r="O74" s="8"/>
-      <c r="P74" s="35"/>
-      <c r="Q74" s="35"/>
-      <c r="R74" s="35"/>
-      <c r="S74" s="35"/>
-      <c r="T74" s="35"/>
+      <c r="P74" s="32"/>
+      <c r="Q74" s="32"/>
+      <c r="R74" s="32"/>
+      <c r="S74" s="32"/>
+      <c r="T74" s="32"/>
       <c r="U74" s="8"/>
       <c r="V74" s="8"/>
       <c r="W74" s="8"/>
@@ -5893,25 +5893,25 @@
       <c r="AK74" s="8"/>
     </row>
     <row r="75" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
       <c r="F75" s="8"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
-      <c r="I75" s="35"/>
-      <c r="J75" s="35"/>
-      <c r="K75" s="35"/>
-      <c r="L75" s="35"/>
-      <c r="M75" s="35"/>
-      <c r="N75" s="35"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="32"/>
+      <c r="K75" s="32"/>
+      <c r="L75" s="32"/>
+      <c r="M75" s="32"/>
+      <c r="N75" s="32"/>
       <c r="O75" s="8"/>
-      <c r="P75" s="35"/>
-      <c r="Q75" s="35"/>
-      <c r="R75" s="35"/>
-      <c r="S75" s="35"/>
-      <c r="T75" s="35"/>
+      <c r="P75" s="32"/>
+      <c r="Q75" s="32"/>
+      <c r="R75" s="32"/>
+      <c r="S75" s="32"/>
+      <c r="T75" s="32"/>
       <c r="U75" s="8"/>
       <c r="V75" s="8"/>
       <c r="W75" s="8"/>
@@ -5935,25 +5935,25 @@
       <c r="AK75" s="8"/>
     </row>
     <row r="76" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
       <c r="F76" s="8"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="35"/>
-      <c r="I76" s="35"/>
-      <c r="J76" s="35"/>
-      <c r="K76" s="35"/>
-      <c r="L76" s="35"/>
-      <c r="M76" s="35"/>
-      <c r="N76" s="35"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="32"/>
+      <c r="J76" s="32"/>
+      <c r="K76" s="32"/>
+      <c r="L76" s="32"/>
+      <c r="M76" s="32"/>
+      <c r="N76" s="32"/>
       <c r="O76" s="8"/>
-      <c r="P76" s="35"/>
-      <c r="Q76" s="35"/>
-      <c r="R76" s="35"/>
-      <c r="S76" s="35"/>
-      <c r="T76" s="35"/>
+      <c r="P76" s="32"/>
+      <c r="Q76" s="32"/>
+      <c r="R76" s="32"/>
+      <c r="S76" s="32"/>
+      <c r="T76" s="32"/>
       <c r="U76" s="8"/>
       <c r="V76" s="8"/>
       <c r="W76" s="8"/>
@@ -5977,25 +5977,25 @@
       <c r="AK76" s="8"/>
     </row>
     <row r="77" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="35"/>
-      <c r="I77" s="35"/>
-      <c r="J77" s="35"/>
-      <c r="K77" s="35"/>
-      <c r="L77" s="35"/>
-      <c r="M77" s="35"/>
-      <c r="N77" s="35"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="32"/>
+      <c r="K77" s="32"/>
+      <c r="L77" s="32"/>
+      <c r="M77" s="32"/>
+      <c r="N77" s="32"/>
       <c r="O77" s="8"/>
-      <c r="P77" s="35"/>
-      <c r="Q77" s="35"/>
-      <c r="R77" s="35"/>
-      <c r="S77" s="35"/>
-      <c r="T77" s="35"/>
+      <c r="P77" s="32"/>
+      <c r="Q77" s="32"/>
+      <c r="R77" s="32"/>
+      <c r="S77" s="32"/>
+      <c r="T77" s="32"/>
       <c r="U77" s="8"/>
       <c r="V77" s="8"/>
       <c r="W77" s="8"/>
@@ -6019,25 +6019,25 @@
       <c r="AK77" s="8"/>
     </row>
     <row r="78" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
       <c r="F78" s="8"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="35"/>
-      <c r="I78" s="35"/>
-      <c r="J78" s="35"/>
-      <c r="K78" s="35"/>
-      <c r="L78" s="35"/>
-      <c r="M78" s="35"/>
-      <c r="N78" s="35"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="32"/>
+      <c r="J78" s="32"/>
+      <c r="K78" s="32"/>
+      <c r="L78" s="32"/>
+      <c r="M78" s="32"/>
+      <c r="N78" s="32"/>
       <c r="O78" s="8"/>
-      <c r="P78" s="35"/>
-      <c r="Q78" s="35"/>
-      <c r="R78" s="35"/>
-      <c r="S78" s="35"/>
-      <c r="T78" s="35"/>
+      <c r="P78" s="32"/>
+      <c r="Q78" s="32"/>
+      <c r="R78" s="32"/>
+      <c r="S78" s="32"/>
+      <c r="T78" s="32"/>
       <c r="U78" s="8"/>
       <c r="V78" s="8"/>
       <c r="W78" s="8"/>
@@ -6075,11 +6075,11 @@
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
       <c r="O79" s="8"/>
-      <c r="P79" s="35"/>
-      <c r="Q79" s="35"/>
-      <c r="R79" s="35"/>
-      <c r="S79" s="35"/>
-      <c r="T79" s="35"/>
+      <c r="P79" s="32"/>
+      <c r="Q79" s="32"/>
+      <c r="R79" s="32"/>
+      <c r="S79" s="32"/>
+      <c r="T79" s="32"/>
       <c r="U79" s="8"/>
       <c r="V79" s="8"/>
       <c r="W79" s="8"/>
@@ -6117,11 +6117,11 @@
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
       <c r="O80" s="8"/>
-      <c r="P80" s="35"/>
-      <c r="Q80" s="35"/>
-      <c r="R80" s="35"/>
-      <c r="S80" s="35"/>
-      <c r="T80" s="35"/>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="32"/>
+      <c r="R80" s="32"/>
+      <c r="S80" s="32"/>
+      <c r="T80" s="32"/>
       <c r="U80" s="8"/>
       <c r="V80" s="8"/>
       <c r="W80" s="8"/>
@@ -6187,15 +6187,15 @@
       <c r="AK81" s="8"/>
     </row>
     <row r="82" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B82" s="25" t="s">
+      <c r="B82" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25" t="s">
+      <c r="C82" s="39"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="F82" s="25"/>
+      <c r="F82" s="39"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
@@ -6233,11 +6233,11 @@
       <c r="AK82" s="8"/>
     </row>
     <row r="83" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
@@ -6278,16 +6278,16 @@
       <c r="B84" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="40" t="e">
+      <c r="C84" s="24" t="e">
         <f>AG19</f>
         <v>#N/A</v>
       </c>
-      <c r="D84" s="41"/>
-      <c r="E84" s="42" t="e">
+      <c r="D84" s="25"/>
+      <c r="E84" s="23" t="e">
         <f>_xlfn.RANK.EQ(C84,$C$84:$D$97)</f>
         <v>#N/A</v>
       </c>
-      <c r="F84" s="42"/>
+      <c r="F84" s="23"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
@@ -6328,16 +6328,16 @@
       <c r="B85" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="40" t="e">
+      <c r="C85" s="24" t="e">
         <f t="shared" ref="C85:C98" si="2">AG20</f>
         <v>#N/A</v>
       </c>
-      <c r="D85" s="41"/>
-      <c r="E85" s="42" t="e">
+      <c r="D85" s="25"/>
+      <c r="E85" s="23" t="e">
         <f t="shared" ref="E85:E98" si="3">_xlfn.RANK.EQ(C85,$C$84:$D$97)</f>
         <v>#N/A</v>
       </c>
-      <c r="F85" s="42"/>
+      <c r="F85" s="23"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
@@ -6378,16 +6378,16 @@
       <c r="B86" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="40" t="e">
+      <c r="C86" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D86" s="41"/>
-      <c r="E86" s="42" t="e">
+      <c r="D86" s="25"/>
+      <c r="E86" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F86" s="42"/>
+      <c r="F86" s="23"/>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
@@ -6428,16 +6428,16 @@
       <c r="B87" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="40" t="e">
+      <c r="C87" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D87" s="41"/>
-      <c r="E87" s="42" t="e">
+      <c r="D87" s="25"/>
+      <c r="E87" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F87" s="42"/>
+      <c r="F87" s="23"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
@@ -6478,16 +6478,16 @@
       <c r="B88" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="40" t="e">
+      <c r="C88" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D88" s="41"/>
-      <c r="E88" s="42" t="e">
+      <c r="D88" s="25"/>
+      <c r="E88" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F88" s="42"/>
+      <c r="F88" s="23"/>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
@@ -6528,32 +6528,32 @@
       <c r="B89" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C89" s="40" t="e">
+      <c r="C89" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D89" s="41"/>
-      <c r="E89" s="42" t="e">
+      <c r="D89" s="25"/>
+      <c r="E89" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F89" s="42"/>
+      <c r="F89" s="23"/>
       <c r="G89" s="8"/>
-      <c r="H89" s="46" t="s">
+      <c r="H89" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="I89" s="47"/>
-      <c r="J89" s="47"/>
-      <c r="K89" s="47"/>
-      <c r="L89" s="47"/>
-      <c r="M89" s="47"/>
-      <c r="N89" s="47"/>
-      <c r="O89" s="47"/>
-      <c r="P89" s="47"/>
-      <c r="Q89" s="47"/>
-      <c r="R89" s="47"/>
-      <c r="S89" s="47"/>
-      <c r="T89" s="47"/>
+      <c r="I89" s="27"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="27"/>
+      <c r="M89" s="27"/>
+      <c r="N89" s="27"/>
+      <c r="O89" s="27"/>
+      <c r="P89" s="27"/>
+      <c r="Q89" s="27"/>
+      <c r="R89" s="27"/>
+      <c r="S89" s="27"/>
+      <c r="T89" s="27"/>
       <c r="U89" s="8"/>
       <c r="V89" s="8"/>
       <c r="W89" s="8"/>
@@ -6580,30 +6580,30 @@
       <c r="B90" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C90" s="40" t="e">
+      <c r="C90" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D90" s="41"/>
-      <c r="E90" s="42" t="e">
+      <c r="D90" s="25"/>
+      <c r="E90" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F90" s="42"/>
+      <c r="F90" s="23"/>
       <c r="G90" s="8"/>
-      <c r="H90" s="47"/>
-      <c r="I90" s="47"/>
-      <c r="J90" s="47"/>
-      <c r="K90" s="47"/>
-      <c r="L90" s="47"/>
-      <c r="M90" s="47"/>
-      <c r="N90" s="47"/>
-      <c r="O90" s="47"/>
-      <c r="P90" s="47"/>
-      <c r="Q90" s="47"/>
-      <c r="R90" s="47"/>
-      <c r="S90" s="47"/>
-      <c r="T90" s="47"/>
+      <c r="H90" s="27"/>
+      <c r="I90" s="27"/>
+      <c r="J90" s="27"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="27"/>
+      <c r="M90" s="27"/>
+      <c r="N90" s="27"/>
+      <c r="O90" s="27"/>
+      <c r="P90" s="27"/>
+      <c r="Q90" s="27"/>
+      <c r="R90" s="27"/>
+      <c r="S90" s="27"/>
+      <c r="T90" s="27"/>
       <c r="U90" s="8"/>
       <c r="V90" s="8"/>
       <c r="W90" s="8"/>
@@ -6630,30 +6630,30 @@
       <c r="B91" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C91" s="40" t="e">
+      <c r="C91" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D91" s="41"/>
-      <c r="E91" s="42" t="e">
+      <c r="D91" s="25"/>
+      <c r="E91" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F91" s="42"/>
+      <c r="F91" s="23"/>
       <c r="G91" s="8"/>
-      <c r="H91" s="47"/>
-      <c r="I91" s="47"/>
-      <c r="J91" s="47"/>
-      <c r="K91" s="47"/>
-      <c r="L91" s="47"/>
-      <c r="M91" s="47"/>
-      <c r="N91" s="47"/>
-      <c r="O91" s="47"/>
-      <c r="P91" s="47"/>
-      <c r="Q91" s="47"/>
-      <c r="R91" s="47"/>
-      <c r="S91" s="47"/>
-      <c r="T91" s="47"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="27"/>
+      <c r="M91" s="27"/>
+      <c r="N91" s="27"/>
+      <c r="O91" s="27"/>
+      <c r="P91" s="27"/>
+      <c r="Q91" s="27"/>
+      <c r="R91" s="27"/>
+      <c r="S91" s="27"/>
+      <c r="T91" s="27"/>
       <c r="U91" s="8"/>
       <c r="V91" s="8"/>
       <c r="W91" s="8"/>
@@ -6680,30 +6680,30 @@
       <c r="B92" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="40" t="e">
+      <c r="C92" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D92" s="41"/>
-      <c r="E92" s="42" t="e">
+      <c r="D92" s="25"/>
+      <c r="E92" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F92" s="42"/>
+      <c r="F92" s="23"/>
       <c r="G92" s="8"/>
-      <c r="H92" s="47"/>
-      <c r="I92" s="47"/>
-      <c r="J92" s="47"/>
-      <c r="K92" s="47"/>
-      <c r="L92" s="47"/>
-      <c r="M92" s="47"/>
-      <c r="N92" s="47"/>
-      <c r="O92" s="47"/>
-      <c r="P92" s="47"/>
-      <c r="Q92" s="47"/>
-      <c r="R92" s="47"/>
-      <c r="S92" s="47"/>
-      <c r="T92" s="47"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="27"/>
+      <c r="M92" s="27"/>
+      <c r="N92" s="27"/>
+      <c r="O92" s="27"/>
+      <c r="P92" s="27"/>
+      <c r="Q92" s="27"/>
+      <c r="R92" s="27"/>
+      <c r="S92" s="27"/>
+      <c r="T92" s="27"/>
       <c r="U92" s="8"/>
       <c r="V92" s="8"/>
       <c r="W92" s="8"/>
@@ -6730,30 +6730,30 @@
       <c r="B93" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="40" t="e">
+      <c r="C93" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D93" s="41"/>
-      <c r="E93" s="42" t="e">
+      <c r="D93" s="25"/>
+      <c r="E93" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F93" s="42"/>
+      <c r="F93" s="23"/>
       <c r="G93" s="8"/>
-      <c r="H93" s="47"/>
-      <c r="I93" s="47"/>
-      <c r="J93" s="47"/>
-      <c r="K93" s="47"/>
-      <c r="L93" s="47"/>
-      <c r="M93" s="47"/>
-      <c r="N93" s="47"/>
-      <c r="O93" s="47"/>
-      <c r="P93" s="47"/>
-      <c r="Q93" s="47"/>
-      <c r="R93" s="47"/>
-      <c r="S93" s="47"/>
-      <c r="T93" s="47"/>
+      <c r="H93" s="27"/>
+      <c r="I93" s="27"/>
+      <c r="J93" s="27"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="27"/>
+      <c r="M93" s="27"/>
+      <c r="N93" s="27"/>
+      <c r="O93" s="27"/>
+      <c r="P93" s="27"/>
+      <c r="Q93" s="27"/>
+      <c r="R93" s="27"/>
+      <c r="S93" s="27"/>
+      <c r="T93" s="27"/>
       <c r="U93" s="8"/>
       <c r="V93" s="8"/>
       <c r="W93" s="8"/>
@@ -6780,30 +6780,30 @@
       <c r="B94" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="40" t="e">
+      <c r="C94" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D94" s="41"/>
-      <c r="E94" s="42" t="e">
+      <c r="D94" s="25"/>
+      <c r="E94" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F94" s="42"/>
+      <c r="F94" s="23"/>
       <c r="G94" s="8"/>
-      <c r="H94" s="47"/>
-      <c r="I94" s="47"/>
-      <c r="J94" s="47"/>
-      <c r="K94" s="47"/>
-      <c r="L94" s="47"/>
-      <c r="M94" s="47"/>
-      <c r="N94" s="47"/>
-      <c r="O94" s="47"/>
-      <c r="P94" s="47"/>
-      <c r="Q94" s="47"/>
-      <c r="R94" s="47"/>
-      <c r="S94" s="47"/>
-      <c r="T94" s="47"/>
+      <c r="H94" s="27"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="27"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="27"/>
+      <c r="M94" s="27"/>
+      <c r="N94" s="27"/>
+      <c r="O94" s="27"/>
+      <c r="P94" s="27"/>
+      <c r="Q94" s="27"/>
+      <c r="R94" s="27"/>
+      <c r="S94" s="27"/>
+      <c r="T94" s="27"/>
       <c r="U94" s="8"/>
       <c r="V94" s="8"/>
       <c r="W94" s="8"/>
@@ -6830,30 +6830,30 @@
       <c r="B95" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="40" t="e">
+      <c r="C95" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D95" s="41"/>
-      <c r="E95" s="42" t="e">
+      <c r="D95" s="25"/>
+      <c r="E95" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F95" s="42"/>
+      <c r="F95" s="23"/>
       <c r="G95" s="8"/>
-      <c r="H95" s="47"/>
-      <c r="I95" s="47"/>
-      <c r="J95" s="47"/>
-      <c r="K95" s="47"/>
-      <c r="L95" s="47"/>
-      <c r="M95" s="47"/>
-      <c r="N95" s="47"/>
-      <c r="O95" s="47"/>
-      <c r="P95" s="47"/>
-      <c r="Q95" s="47"/>
-      <c r="R95" s="47"/>
-      <c r="S95" s="47"/>
-      <c r="T95" s="47"/>
+      <c r="H95" s="27"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="27"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="27"/>
+      <c r="N95" s="27"/>
+      <c r="O95" s="27"/>
+      <c r="P95" s="27"/>
+      <c r="Q95" s="27"/>
+      <c r="R95" s="27"/>
+      <c r="S95" s="27"/>
+      <c r="T95" s="27"/>
       <c r="U95" s="8"/>
       <c r="V95" s="8"/>
       <c r="W95" s="8"/>
@@ -6880,16 +6880,16 @@
       <c r="B96" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C96" s="40" t="e">
+      <c r="C96" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D96" s="41"/>
-      <c r="E96" s="42" t="e">
+      <c r="D96" s="25"/>
+      <c r="E96" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="42"/>
+      <c r="F96" s="23"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
@@ -6930,16 +6930,16 @@
       <c r="B97" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C97" s="40" t="e">
+      <c r="C97" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D97" s="41"/>
-      <c r="E97" s="42" t="e">
+      <c r="D97" s="25"/>
+      <c r="E97" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F97" s="42"/>
+      <c r="F97" s="23"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
       <c r="I97" s="8"/>
@@ -6980,32 +6980,32 @@
       <c r="B98" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C98" s="40" t="e">
+      <c r="C98" s="24" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D98" s="41"/>
-      <c r="E98" s="42" t="e">
+      <c r="D98" s="25"/>
+      <c r="E98" s="23" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F98" s="42"/>
+      <c r="F98" s="23"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
-      <c r="I98" s="48" t="s">
+      <c r="I98" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="J98" s="49"/>
-      <c r="K98" s="49"/>
-      <c r="L98" s="49"/>
-      <c r="M98" s="49"/>
-      <c r="N98" s="49"/>
-      <c r="O98" s="49"/>
-      <c r="P98" s="49"/>
-      <c r="Q98" s="49"/>
-      <c r="R98" s="49"/>
-      <c r="S98" s="49"/>
-      <c r="T98" s="49"/>
+      <c r="J98" s="29"/>
+      <c r="K98" s="29"/>
+      <c r="L98" s="29"/>
+      <c r="M98" s="29"/>
+      <c r="N98" s="29"/>
+      <c r="O98" s="29"/>
+      <c r="P98" s="29"/>
+      <c r="Q98" s="29"/>
+      <c r="R98" s="29"/>
+      <c r="S98" s="29"/>
+      <c r="T98" s="29"/>
       <c r="U98" s="8"/>
       <c r="V98" s="8"/>
       <c r="W98" s="8"/>
@@ -7036,18 +7036,18 @@
       <c r="F99" s="8"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
-      <c r="I99" s="49"/>
-      <c r="J99" s="49"/>
-      <c r="K99" s="49"/>
-      <c r="L99" s="49"/>
-      <c r="M99" s="49"/>
-      <c r="N99" s="49"/>
-      <c r="O99" s="49"/>
-      <c r="P99" s="49"/>
-      <c r="Q99" s="49"/>
-      <c r="R99" s="49"/>
-      <c r="S99" s="49"/>
-      <c r="T99" s="49"/>
+      <c r="I99" s="29"/>
+      <c r="J99" s="29"/>
+      <c r="K99" s="29"/>
+      <c r="L99" s="29"/>
+      <c r="M99" s="29"/>
+      <c r="N99" s="29"/>
+      <c r="O99" s="29"/>
+      <c r="P99" s="29"/>
+      <c r="Q99" s="29"/>
+      <c r="R99" s="29"/>
+      <c r="S99" s="29"/>
+      <c r="T99" s="29"/>
       <c r="U99" s="8"/>
       <c r="V99" s="8"/>
       <c r="W99" s="8"/>
@@ -7078,18 +7078,18 @@
       <c r="F100" s="8"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
-      <c r="I100" s="49"/>
-      <c r="J100" s="49"/>
-      <c r="K100" s="49"/>
-      <c r="L100" s="49"/>
-      <c r="M100" s="49"/>
-      <c r="N100" s="49"/>
-      <c r="O100" s="49"/>
-      <c r="P100" s="49"/>
-      <c r="Q100" s="49"/>
-      <c r="R100" s="49"/>
-      <c r="S100" s="49"/>
-      <c r="T100" s="49"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
+      <c r="K100" s="29"/>
+      <c r="L100" s="29"/>
+      <c r="M100" s="29"/>
+      <c r="N100" s="29"/>
+      <c r="O100" s="29"/>
+      <c r="P100" s="29"/>
+      <c r="Q100" s="29"/>
+      <c r="R100" s="29"/>
+      <c r="S100" s="29"/>
+      <c r="T100" s="29"/>
       <c r="U100" s="8"/>
       <c r="V100" s="8"/>
       <c r="W100" s="8"/>
@@ -7120,18 +7120,18 @@
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
       <c r="H101" s="8"/>
-      <c r="I101" s="49"/>
-      <c r="J101" s="49"/>
-      <c r="K101" s="49"/>
-      <c r="L101" s="49"/>
-      <c r="M101" s="49"/>
-      <c r="N101" s="49"/>
-      <c r="O101" s="49"/>
-      <c r="P101" s="49"/>
-      <c r="Q101" s="49"/>
-      <c r="R101" s="49"/>
-      <c r="S101" s="49"/>
-      <c r="T101" s="49"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="29"/>
+      <c r="N101" s="29"/>
+      <c r="O101" s="29"/>
+      <c r="P101" s="29"/>
+      <c r="Q101" s="29"/>
+      <c r="R101" s="29"/>
+      <c r="S101" s="29"/>
+      <c r="T101" s="29"/>
       <c r="U101" s="8"/>
       <c r="V101" s="8"/>
       <c r="W101" s="8"/>
@@ -7163,19 +7163,19 @@
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
-      <c r="J102" s="50" t="s">
+      <c r="J102" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="K102" s="51"/>
-      <c r="L102" s="51"/>
-      <c r="M102" s="51"/>
-      <c r="N102" s="51"/>
-      <c r="O102" s="51"/>
-      <c r="P102" s="51"/>
-      <c r="Q102" s="51"/>
-      <c r="R102" s="51"/>
-      <c r="S102" s="51"/>
-      <c r="T102" s="51"/>
+      <c r="K102" s="31"/>
+      <c r="L102" s="31"/>
+      <c r="M102" s="31"/>
+      <c r="N102" s="31"/>
+      <c r="O102" s="31"/>
+      <c r="P102" s="31"/>
+      <c r="Q102" s="31"/>
+      <c r="R102" s="31"/>
+      <c r="S102" s="31"/>
+      <c r="T102" s="31"/>
       <c r="U102" s="8"/>
       <c r="V102" s="8"/>
       <c r="W102" s="8"/>
@@ -7207,17 +7207,17 @@
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
-      <c r="J103" s="51"/>
-      <c r="K103" s="51"/>
-      <c r="L103" s="51"/>
-      <c r="M103" s="51"/>
-      <c r="N103" s="51"/>
-      <c r="O103" s="51"/>
-      <c r="P103" s="51"/>
-      <c r="Q103" s="51"/>
-      <c r="R103" s="51"/>
-      <c r="S103" s="51"/>
-      <c r="T103" s="51"/>
+      <c r="J103" s="31"/>
+      <c r="K103" s="31"/>
+      <c r="L103" s="31"/>
+      <c r="M103" s="31"/>
+      <c r="N103" s="31"/>
+      <c r="O103" s="31"/>
+      <c r="P103" s="31"/>
+      <c r="Q103" s="31"/>
+      <c r="R103" s="31"/>
+      <c r="S103" s="31"/>
+      <c r="T103" s="31"/>
       <c r="U103" s="8"/>
       <c r="V103" s="8"/>
       <c r="W103" s="8"/>
@@ -7249,17 +7249,17 @@
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
-      <c r="J104" s="51"/>
-      <c r="K104" s="51"/>
-      <c r="L104" s="51"/>
-      <c r="M104" s="51"/>
-      <c r="N104" s="51"/>
-      <c r="O104" s="51"/>
-      <c r="P104" s="51"/>
-      <c r="Q104" s="51"/>
-      <c r="R104" s="51"/>
-      <c r="S104" s="51"/>
-      <c r="T104" s="51"/>
+      <c r="J104" s="31"/>
+      <c r="K104" s="31"/>
+      <c r="L104" s="31"/>
+      <c r="M104" s="31"/>
+      <c r="N104" s="31"/>
+      <c r="O104" s="31"/>
+      <c r="P104" s="31"/>
+      <c r="Q104" s="31"/>
+      <c r="R104" s="31"/>
+      <c r="S104" s="31"/>
+      <c r="T104" s="31"/>
       <c r="U104" s="8"/>
       <c r="V104" s="8"/>
       <c r="W104" s="8"/>
@@ -8023,14 +8023,64 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="S26:W28"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="B5:X7"/>
+    <mergeCell ref="B1:X2"/>
+    <mergeCell ref="B4:X4"/>
+    <mergeCell ref="B8:X8"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B9:X10"/>
+    <mergeCell ref="B11:X12"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B13:X14"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="Q40:T40"/>
+    <mergeCell ref="V39:X39"/>
+    <mergeCell ref="V40:X40"/>
+    <mergeCell ref="Q39:T39"/>
+    <mergeCell ref="B34:T35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="G40:N40"/>
+    <mergeCell ref="G39:N39"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B57:E67"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="G69:N69"/>
+    <mergeCell ref="P69:T69"/>
+    <mergeCell ref="B70:E78"/>
+    <mergeCell ref="G70:N78"/>
+    <mergeCell ref="P57:T67"/>
+    <mergeCell ref="G57:N67"/>
+    <mergeCell ref="P70:T80"/>
+    <mergeCell ref="B82:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E82:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="P56:T56"/>
+    <mergeCell ref="V57:X67"/>
+    <mergeCell ref="V56:X56"/>
+    <mergeCell ref="V42:X42"/>
+    <mergeCell ref="V43:X51"/>
+    <mergeCell ref="Q42:T42"/>
+    <mergeCell ref="Q43:T52"/>
+    <mergeCell ref="B43:E54"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="G43:N54"/>
+    <mergeCell ref="G42:N42"/>
+    <mergeCell ref="G56:N56"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="H89:T95"/>
     <mergeCell ref="I98:T101"/>
@@ -8047,64 +8097,14 @@
     <mergeCell ref="E94:F94"/>
     <mergeCell ref="E95:F95"/>
     <mergeCell ref="E96:F96"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="B43:E54"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="G43:N54"/>
-    <mergeCell ref="G42:N42"/>
-    <mergeCell ref="G56:N56"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="P56:T56"/>
-    <mergeCell ref="V57:X67"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="V42:X42"/>
-    <mergeCell ref="V43:X51"/>
-    <mergeCell ref="Q42:T42"/>
-    <mergeCell ref="Q43:T52"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="B57:E67"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="G69:N69"/>
-    <mergeCell ref="P69:T69"/>
-    <mergeCell ref="B70:E78"/>
-    <mergeCell ref="G70:N78"/>
-    <mergeCell ref="P57:T67"/>
-    <mergeCell ref="G57:N67"/>
-    <mergeCell ref="P70:T80"/>
-    <mergeCell ref="B82:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E82:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="Q40:T40"/>
-    <mergeCell ref="V39:X39"/>
-    <mergeCell ref="V40:X40"/>
-    <mergeCell ref="Q39:T39"/>
-    <mergeCell ref="B34:T35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="G40:N40"/>
-    <mergeCell ref="G39:N39"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="S26:W28"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="B5:X7"/>
-    <mergeCell ref="B1:X2"/>
-    <mergeCell ref="B4:X4"/>
-    <mergeCell ref="B8:X8"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B9:X10"/>
-    <mergeCell ref="B11:X12"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B13:X14"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
   </mergeCells>
   <conditionalFormatting sqref="C84:D98">
     <cfRule type="colorScale" priority="1">
@@ -8543,10 +8543,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD34DB8-C9A5-4D57-A0EC-7EAD29CA4537}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8554,6 +8554,12 @@
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -8672,20 +8678,6 @@
       </c>
       <c r="S2">
         <v>6.1904761904761907</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -8842,12 +8834,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9029,19 +9022,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E55394AD-EAD7-4DB0-8A63-1FFADDFE8C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{868C143E-6D51-4467-8AC0-C13BFF0C5CF6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9066,17 +9066,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{868C143E-6D51-4467-8AC0-C13BFF0C5CF6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E55394AD-EAD7-4DB0-8A63-1FFADDFE8C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added criteria grade for elec and smr
</commit_message>
<xml_diff>
--- a/Criteria Ranking.xlsx
+++ b/Criteria Ranking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matis\Desktop\Aalto S1\Advanced Energy Project\SMR-X-H2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F435461-AB11-41E9-980E-C5B96A54F63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78BEAB1-F5B9-4A8A-90F7-2EC192F9835F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -1226,68 +1226,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1311,6 +1260,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2061,31 +2061,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
       <c r="Y1" s="18"/>
       <c r="Z1" s="8"/>
       <c r="AA1" s="8"/>
@@ -2101,29 +2101,29 @@
       <c r="AK1" s="8"/>
     </row>
     <row r="2" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
       <c r="Y2" s="18"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
@@ -2139,10 +2139,10 @@
       <c r="AK2" s="8"/>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2179,31 +2179,31 @@
       <c r="AK3" s="8"/>
     </row>
     <row r="4" spans="2:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="18"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
@@ -2219,31 +2219,31 @@
       <c r="AK4" s="8"/>
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
       <c r="Y5" s="18"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
@@ -2259,29 +2259,29 @@
       <c r="AK5" s="8"/>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
       <c r="Y6" s="18"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
@@ -2297,29 +2297,29 @@
       <c r="AK6" s="8"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
       <c r="Y7" s="18"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
@@ -2335,31 +2335,31 @@
       <c r="AK7" s="8"/>
     </row>
     <row r="8" spans="2:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
       <c r="Y8" s="18"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
@@ -2375,31 +2375,31 @@
       <c r="AK8" s="8"/>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="42"/>
-      <c r="X9" s="42"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
       <c r="Y9" s="18"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
@@ -2415,29 +2415,29 @@
       <c r="AK9" s="8"/>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
       <c r="Y10" s="18"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8"/>
@@ -2453,31 +2453,31 @@
       <c r="AK10" s="8"/>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
       <c r="Y11" s="18"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
@@ -2493,29 +2493,29 @@
       <c r="AK11" s="8"/>
     </row>
     <row r="12" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
       <c r="Y12" s="18"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
@@ -2531,31 +2531,31 @@
       <c r="AK12" s="8"/>
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="51"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="34"/>
       <c r="Y13" s="18"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
@@ -2571,29 +2571,29 @@
       <c r="AK13" s="8"/>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="51"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="34"/>
       <c r="Y14" s="18"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
@@ -2650,32 +2650,32 @@
       <c r="B16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="42" t="s">
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="48" t="s">
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="42" t="s">
+      <c r="L16" s="31"/>
+      <c r="M16" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="48" t="s">
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -2797,12 +2797,12 @@
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="8"/>
-      <c r="T18" s="39" t="s">
+      <c r="T18" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="U18" s="39"/>
-      <c r="V18" s="39"/>
-      <c r="W18" s="39"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="18"/>
       <c r="Z18" s="8"/>
@@ -3468,11 +3468,11 @@
         <v>26</v>
       </c>
       <c r="R26" s="8"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="42"/>
-      <c r="W26" s="42"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
       <c r="X26" s="8"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="8"/>
@@ -3556,11 +3556,11 @@
         <v>26</v>
       </c>
       <c r="R27" s="8"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="42"/>
-      <c r="W27" s="42"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
       <c r="X27" s="8"/>
       <c r="Y27" s="18"/>
       <c r="Z27" s="8"/>
@@ -3643,11 +3643,11 @@
         <v>26</v>
       </c>
       <c r="R28" s="8"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
-      <c r="U28" s="42"/>
-      <c r="V28" s="42"/>
-      <c r="W28" s="42"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
       <c r="X28" s="8"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="8"/>
@@ -4124,27 +4124,27 @@
       <c r="AK33" s="8"/>
     </row>
     <row r="34" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
+      <c r="T34" s="38"/>
       <c r="U34" s="8"/>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
@@ -4168,25 +4168,25 @@
       <c r="AK34" s="8"/>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="40"/>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="40"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="40"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="38"/>
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
@@ -4248,10 +4248,10 @@
       <c r="AK36" s="8"/>
     </row>
     <row r="37" spans="2:37" ht="21" x14ac:dyDescent="0.4">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="43"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
@@ -4339,37 +4339,37 @@
       <c r="AK38" s="8"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="41" t="s">
+      <c r="G39" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="41"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
       <c r="O39" s="16"/>
       <c r="P39" s="8"/>
-      <c r="Q39" s="34" t="s">
+      <c r="Q39" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="37"/>
       <c r="U39" s="8"/>
-      <c r="V39" s="35" t="s">
+      <c r="V39" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="W39" s="35"/>
-      <c r="X39" s="35"/>
+      <c r="W39" s="36"/>
+      <c r="X39" s="36"/>
       <c r="Y39" s="18"/>
       <c r="Z39" s="8"/>
       <c r="AA39" s="8" t="s">
@@ -4389,37 +4389,37 @@
       <c r="AK39" s="8"/>
     </row>
     <row r="40" spans="2:37" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="32" t="s">
+      <c r="G40" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
       <c r="O40" s="13"/>
       <c r="P40" s="8"/>
-      <c r="Q40" s="32" t="s">
+      <c r="Q40" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="R40" s="32"/>
-      <c r="S40" s="32"/>
-      <c r="T40" s="32"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
       <c r="U40" s="13"/>
-      <c r="V40" s="32" t="s">
+      <c r="V40" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="W40" s="32"/>
-      <c r="X40" s="32"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
       <c r="Y40" s="18"/>
       <c r="Z40" s="8"/>
       <c r="AA40" s="8" t="s">
@@ -4479,37 +4479,37 @@
       <c r="AK41" s="8"/>
     </row>
     <row r="42" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="34" t="s">
+      <c r="G42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
       <c r="O42" s="1"/>
       <c r="P42" s="8"/>
-      <c r="Q42" s="35" t="s">
+      <c r="Q42" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="R42" s="35"/>
-      <c r="S42" s="35"/>
-      <c r="T42" s="35"/>
+      <c r="R42" s="36"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="36"/>
       <c r="U42" s="8"/>
-      <c r="V42" s="35" t="s">
+      <c r="V42" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="W42" s="35"/>
-      <c r="X42" s="35"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
       <c r="Y42" s="18"/>
       <c r="Z42" s="8"/>
       <c r="AA42" s="8" t="s">
@@ -4527,37 +4527,37 @@
       <c r="AK42" s="8"/>
     </row>
     <row r="43" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="32" t="s">
+      <c r="G43" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
       <c r="O43" s="15"/>
       <c r="P43" s="8"/>
-      <c r="Q43" s="36" t="s">
+      <c r="Q43" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="R43" s="37"/>
-      <c r="S43" s="37"/>
-      <c r="T43" s="37"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
       <c r="U43" s="8"/>
-      <c r="V43" s="36" t="s">
+      <c r="V43" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="W43" s="37"/>
-      <c r="X43" s="37"/>
+      <c r="W43" s="44"/>
+      <c r="X43" s="44"/>
       <c r="Y43" s="18"/>
       <c r="Z43" s="8"/>
       <c r="AA43" s="8" t="s">
@@ -4577,29 +4577,29 @@
       <c r="AK43" s="8"/>
     </row>
     <row r="44" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B44" s="32"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
       <c r="O44" s="15"/>
       <c r="P44" s="8"/>
-      <c r="Q44" s="37"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="37"/>
-      <c r="T44" s="37"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="44"/>
+      <c r="S44" s="44"/>
+      <c r="T44" s="44"/>
       <c r="U44" s="8"/>
-      <c r="V44" s="37"/>
-      <c r="W44" s="37"/>
-      <c r="X44" s="37"/>
+      <c r="V44" s="44"/>
+      <c r="W44" s="44"/>
+      <c r="X44" s="44"/>
       <c r="Y44" s="18"/>
       <c r="Z44" s="8"/>
       <c r="AA44" s="8" t="s">
@@ -4619,29 +4619,29 @@
       <c r="AK44" s="8"/>
     </row>
     <row r="45" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
       <c r="O45" s="15"/>
       <c r="P45" s="8"/>
-      <c r="Q45" s="37"/>
-      <c r="R45" s="37"/>
-      <c r="S45" s="37"/>
-      <c r="T45" s="37"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="44"/>
+      <c r="S45" s="44"/>
+      <c r="T45" s="44"/>
       <c r="U45" s="8"/>
-      <c r="V45" s="37"/>
-      <c r="W45" s="37"/>
-      <c r="X45" s="37"/>
+      <c r="V45" s="44"/>
+      <c r="W45" s="44"/>
+      <c r="X45" s="44"/>
       <c r="Y45" s="18"/>
       <c r="Z45" s="8"/>
       <c r="AA45" s="8" t="s">
@@ -4659,29 +4659,29 @@
       <c r="AK45" s="8"/>
     </row>
     <row r="46" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
       <c r="O46" s="15"/>
       <c r="P46" s="8"/>
-      <c r="Q46" s="37"/>
-      <c r="R46" s="37"/>
-      <c r="S46" s="37"/>
-      <c r="T46" s="37"/>
+      <c r="Q46" s="44"/>
+      <c r="R46" s="44"/>
+      <c r="S46" s="44"/>
+      <c r="T46" s="44"/>
       <c r="U46" s="8"/>
-      <c r="V46" s="37"/>
-      <c r="W46" s="37"/>
-      <c r="X46" s="37"/>
+      <c r="V46" s="44"/>
+      <c r="W46" s="44"/>
+      <c r="X46" s="44"/>
       <c r="Y46" s="18"/>
       <c r="Z46" s="8"/>
       <c r="AA46" s="8" t="s">
@@ -4701,29 +4701,29 @@
       <c r="AK46" s="8"/>
     </row>
     <row r="47" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
       <c r="O47" s="15"/>
       <c r="P47" s="8"/>
-      <c r="Q47" s="37"/>
-      <c r="R47" s="37"/>
-      <c r="S47" s="37"/>
-      <c r="T47" s="37"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="44"/>
+      <c r="S47" s="44"/>
+      <c r="T47" s="44"/>
       <c r="U47" s="8"/>
-      <c r="V47" s="37"/>
-      <c r="W47" s="37"/>
-      <c r="X47" s="37"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="44"/>
+      <c r="X47" s="44"/>
       <c r="Y47" s="18"/>
       <c r="Z47" s="8"/>
       <c r="AA47" s="8" t="s">
@@ -4743,29 +4743,29 @@
       <c r="AK47" s="8"/>
     </row>
     <row r="48" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
       <c r="O48" s="15"/>
       <c r="P48" s="8"/>
-      <c r="Q48" s="37"/>
-      <c r="R48" s="37"/>
-      <c r="S48" s="37"/>
-      <c r="T48" s="37"/>
+      <c r="Q48" s="44"/>
+      <c r="R48" s="44"/>
+      <c r="S48" s="44"/>
+      <c r="T48" s="44"/>
       <c r="U48" s="8"/>
-      <c r="V48" s="37"/>
-      <c r="W48" s="37"/>
-      <c r="X48" s="37"/>
+      <c r="V48" s="44"/>
+      <c r="W48" s="44"/>
+      <c r="X48" s="44"/>
       <c r="Y48" s="18"/>
       <c r="Z48" s="8"/>
       <c r="AA48" s="8" t="s">
@@ -4785,29 +4785,29 @@
       <c r="AK48" s="8"/>
     </row>
     <row r="49" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
       <c r="O49" s="15"/>
       <c r="P49" s="8"/>
-      <c r="Q49" s="37"/>
-      <c r="R49" s="37"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="37"/>
+      <c r="Q49" s="44"/>
+      <c r="R49" s="44"/>
+      <c r="S49" s="44"/>
+      <c r="T49" s="44"/>
       <c r="U49" s="8"/>
-      <c r="V49" s="37"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="37"/>
+      <c r="V49" s="44"/>
+      <c r="W49" s="44"/>
+      <c r="X49" s="44"/>
       <c r="Y49" s="18"/>
       <c r="Z49" s="8"/>
       <c r="AA49" s="8" t="s">
@@ -4827,29 +4827,29 @@
       <c r="AK49" s="8"/>
     </row>
     <row r="50" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
       <c r="O50" s="15"/>
       <c r="P50" s="8"/>
-      <c r="Q50" s="37"/>
-      <c r="R50" s="37"/>
-      <c r="S50" s="37"/>
-      <c r="T50" s="37"/>
+      <c r="Q50" s="44"/>
+      <c r="R50" s="44"/>
+      <c r="S50" s="44"/>
+      <c r="T50" s="44"/>
       <c r="U50" s="8"/>
-      <c r="V50" s="37"/>
-      <c r="W50" s="37"/>
-      <c r="X50" s="37"/>
+      <c r="V50" s="44"/>
+      <c r="W50" s="44"/>
+      <c r="X50" s="44"/>
       <c r="Y50" s="18"/>
       <c r="Z50" s="8"/>
       <c r="AA50" s="8" t="s">
@@ -4869,29 +4869,29 @@
       <c r="AK50" s="8"/>
     </row>
     <row r="51" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
       <c r="O51" s="15"/>
       <c r="P51" s="8"/>
-      <c r="Q51" s="37"/>
-      <c r="R51" s="37"/>
-      <c r="S51" s="37"/>
-      <c r="T51" s="37"/>
+      <c r="Q51" s="44"/>
+      <c r="R51" s="44"/>
+      <c r="S51" s="44"/>
+      <c r="T51" s="44"/>
       <c r="U51" s="8"/>
-      <c r="V51" s="37"/>
-      <c r="W51" s="37"/>
-      <c r="X51" s="37"/>
+      <c r="V51" s="44"/>
+      <c r="W51" s="44"/>
+      <c r="X51" s="44"/>
       <c r="Y51" s="18"/>
       <c r="Z51" s="8"/>
       <c r="AA51" s="8" t="s">
@@ -4911,25 +4911,25 @@
       <c r="AK51" s="8"/>
     </row>
     <row r="52" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
       <c r="O52" s="15"/>
       <c r="P52" s="8"/>
-      <c r="Q52" s="37"/>
-      <c r="R52" s="37"/>
-      <c r="S52" s="37"/>
-      <c r="T52" s="37"/>
+      <c r="Q52" s="44"/>
+      <c r="R52" s="44"/>
+      <c r="S52" s="44"/>
+      <c r="T52" s="44"/>
       <c r="U52" s="8"/>
       <c r="V52" s="8"/>
       <c r="W52" s="8"/>
@@ -4953,19 +4953,19 @@
       <c r="AK52" s="8"/>
     </row>
     <row r="53" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
       <c r="F53" s="8"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
       <c r="O53" s="8"/>
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
@@ -4995,19 +4995,19 @@
       <c r="AK53" s="8"/>
     </row>
     <row r="54" spans="2:37" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
       <c r="O54" s="8"/>
       <c r="P54" s="8"/>
       <c r="Q54" s="8"/>
@@ -5077,37 +5077,37 @@
       <c r="AK55" s="8"/>
     </row>
     <row r="56" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
       <c r="F56" s="8"/>
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
       <c r="O56" s="8"/>
-      <c r="P56" s="35" t="s">
+      <c r="P56" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="Q56" s="35"/>
-      <c r="R56" s="35"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="35"/>
+      <c r="Q56" s="36"/>
+      <c r="R56" s="36"/>
+      <c r="S56" s="36"/>
+      <c r="T56" s="36"/>
       <c r="U56" s="8"/>
-      <c r="V56" s="35" t="s">
+      <c r="V56" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="W56" s="35"/>
-      <c r="X56" s="35"/>
+      <c r="W56" s="36"/>
+      <c r="X56" s="36"/>
       <c r="Y56" s="18"/>
       <c r="Z56" s="8"/>
       <c r="AA56" s="8" t="s">
@@ -5127,37 +5127,37 @@
       <c r="AK56" s="8"/>
     </row>
     <row r="57" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="32" t="s">
+      <c r="G57" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="35"/>
+      <c r="N57" s="35"/>
       <c r="O57" s="8"/>
-      <c r="P57" s="38" t="s">
+      <c r="P57" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="Q57" s="38"/>
-      <c r="R57" s="38"/>
-      <c r="S57" s="38"/>
-      <c r="T57" s="38"/>
+      <c r="Q57" s="26"/>
+      <c r="R57" s="26"/>
+      <c r="S57" s="26"/>
+      <c r="T57" s="26"/>
       <c r="U57" s="8"/>
-      <c r="V57" s="32" t="s">
+      <c r="V57" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="W57" s="32"/>
-      <c r="X57" s="32"/>
+      <c r="W57" s="35"/>
+      <c r="X57" s="35"/>
       <c r="Y57" s="18"/>
       <c r="Z57" s="8"/>
       <c r="AA57" s="8" t="s">
@@ -5177,29 +5177,29 @@
       <c r="AK57" s="8"/>
     </row>
     <row r="58" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="32"/>
-      <c r="N58" s="32"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35"/>
+      <c r="N58" s="35"/>
       <c r="O58" s="8"/>
-      <c r="P58" s="38"/>
-      <c r="Q58" s="38"/>
-      <c r="R58" s="38"/>
-      <c r="S58" s="38"/>
-      <c r="T58" s="38"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
+      <c r="R58" s="26"/>
+      <c r="S58" s="26"/>
+      <c r="T58" s="26"/>
       <c r="U58" s="8"/>
-      <c r="V58" s="32"/>
-      <c r="W58" s="32"/>
-      <c r="X58" s="32"/>
+      <c r="V58" s="35"/>
+      <c r="W58" s="35"/>
+      <c r="X58" s="35"/>
       <c r="Y58" s="18"/>
       <c r="Z58" s="8"/>
       <c r="AA58" s="8" t="s">
@@ -5219,29 +5219,29 @@
       <c r="AK58" s="8"/>
     </row>
     <row r="59" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
       <c r="F59" s="8"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="32"/>
-      <c r="N59" s="32"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
       <c r="O59" s="8"/>
-      <c r="P59" s="38"/>
-      <c r="Q59" s="38"/>
-      <c r="R59" s="38"/>
-      <c r="S59" s="38"/>
-      <c r="T59" s="38"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="26"/>
+      <c r="R59" s="26"/>
+      <c r="S59" s="26"/>
+      <c r="T59" s="26"/>
       <c r="U59" s="8"/>
-      <c r="V59" s="32"/>
-      <c r="W59" s="32"/>
-      <c r="X59" s="32"/>
+      <c r="V59" s="35"/>
+      <c r="W59" s="35"/>
+      <c r="X59" s="35"/>
       <c r="Y59" s="18"/>
       <c r="Z59" s="8"/>
       <c r="AA59" s="8" t="s">
@@ -5261,29 +5261,29 @@
       <c r="AK59" s="8"/>
     </row>
     <row r="60" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
       <c r="F60" s="8"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="32"/>
-      <c r="N60" s="32"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
       <c r="O60" s="8"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="38"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="38"/>
+      <c r="P60" s="26"/>
+      <c r="Q60" s="26"/>
+      <c r="R60" s="26"/>
+      <c r="S60" s="26"/>
+      <c r="T60" s="26"/>
       <c r="U60" s="8"/>
-      <c r="V60" s="32"/>
-      <c r="W60" s="32"/>
-      <c r="X60" s="32"/>
+      <c r="V60" s="35"/>
+      <c r="W60" s="35"/>
+      <c r="X60" s="35"/>
       <c r="Y60" s="18"/>
       <c r="Z60" s="8"/>
       <c r="AA60" s="8" t="s">
@@ -5303,29 +5303,29 @@
       <c r="AK60" s="8"/>
     </row>
     <row r="61" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="35"/>
+      <c r="N61" s="35"/>
       <c r="O61" s="8"/>
-      <c r="P61" s="38"/>
-      <c r="Q61" s="38"/>
-      <c r="R61" s="38"/>
-      <c r="S61" s="38"/>
-      <c r="T61" s="38"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="26"/>
+      <c r="R61" s="26"/>
+      <c r="S61" s="26"/>
+      <c r="T61" s="26"/>
       <c r="U61" s="8"/>
-      <c r="V61" s="32"/>
-      <c r="W61" s="32"/>
-      <c r="X61" s="32"/>
+      <c r="V61" s="35"/>
+      <c r="W61" s="35"/>
+      <c r="X61" s="35"/>
       <c r="Y61" s="18"/>
       <c r="Z61" s="8"/>
       <c r="AA61" s="8" t="s">
@@ -5345,29 +5345,29 @@
       <c r="AK61" s="8"/>
     </row>
     <row r="62" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
       <c r="F62" s="8"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
       <c r="O62" s="8"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="38"/>
-      <c r="R62" s="38"/>
-      <c r="S62" s="38"/>
-      <c r="T62" s="38"/>
+      <c r="P62" s="26"/>
+      <c r="Q62" s="26"/>
+      <c r="R62" s="26"/>
+      <c r="S62" s="26"/>
+      <c r="T62" s="26"/>
       <c r="U62" s="8"/>
-      <c r="V62" s="32"/>
-      <c r="W62" s="32"/>
-      <c r="X62" s="32"/>
+      <c r="V62" s="35"/>
+      <c r="W62" s="35"/>
+      <c r="X62" s="35"/>
       <c r="Y62" s="18"/>
       <c r="Z62" s="8"/>
       <c r="AA62" s="8" t="s">
@@ -5387,29 +5387,29 @@
       <c r="AK62" s="8"/>
     </row>
     <row r="63" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="32"/>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
       <c r="O63" s="8"/>
-      <c r="P63" s="38"/>
-      <c r="Q63" s="38"/>
-      <c r="R63" s="38"/>
-      <c r="S63" s="38"/>
-      <c r="T63" s="38"/>
+      <c r="P63" s="26"/>
+      <c r="Q63" s="26"/>
+      <c r="R63" s="26"/>
+      <c r="S63" s="26"/>
+      <c r="T63" s="26"/>
       <c r="U63" s="8"/>
-      <c r="V63" s="32"/>
-      <c r="W63" s="32"/>
-      <c r="X63" s="32"/>
+      <c r="V63" s="35"/>
+      <c r="W63" s="35"/>
+      <c r="X63" s="35"/>
       <c r="Y63" s="18"/>
       <c r="Z63" s="8"/>
       <c r="AA63" s="8" t="s">
@@ -5429,29 +5429,29 @@
       <c r="AK63" s="8"/>
     </row>
     <row r="64" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B64" s="32"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
-      <c r="J64" s="32"/>
-      <c r="K64" s="32"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="32"/>
-      <c r="N64" s="32"/>
+      <c r="G64" s="35"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="35"/>
+      <c r="N64" s="35"/>
       <c r="O64" s="8"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="38"/>
-      <c r="R64" s="38"/>
-      <c r="S64" s="38"/>
-      <c r="T64" s="38"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="26"/>
+      <c r="R64" s="26"/>
+      <c r="S64" s="26"/>
+      <c r="T64" s="26"/>
       <c r="U64" s="8"/>
-      <c r="V64" s="32"/>
-      <c r="W64" s="32"/>
-      <c r="X64" s="32"/>
+      <c r="V64" s="35"/>
+      <c r="W64" s="35"/>
+      <c r="X64" s="35"/>
       <c r="Y64" s="18"/>
       <c r="Z64" s="8"/>
       <c r="AA64" s="8" t="s">
@@ -5471,29 +5471,29 @@
       <c r="AK64" s="8"/>
     </row>
     <row r="65" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
       <c r="F65" s="8"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
-      <c r="J65" s="32"/>
-      <c r="K65" s="32"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="32"/>
-      <c r="N65" s="32"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="35"/>
       <c r="O65" s="8"/>
-      <c r="P65" s="38"/>
-      <c r="Q65" s="38"/>
-      <c r="R65" s="38"/>
-      <c r="S65" s="38"/>
-      <c r="T65" s="38"/>
+      <c r="P65" s="26"/>
+      <c r="Q65" s="26"/>
+      <c r="R65" s="26"/>
+      <c r="S65" s="26"/>
+      <c r="T65" s="26"/>
       <c r="U65" s="8"/>
-      <c r="V65" s="32"/>
-      <c r="W65" s="32"/>
-      <c r="X65" s="32"/>
+      <c r="V65" s="35"/>
+      <c r="W65" s="35"/>
+      <c r="X65" s="35"/>
       <c r="Y65" s="18"/>
       <c r="Z65" s="8"/>
       <c r="AA65" s="8" t="s">
@@ -5513,29 +5513,29 @@
       <c r="AK65" s="8"/>
     </row>
     <row r="66" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32"/>
-      <c r="K66" s="32"/>
-      <c r="L66" s="32"/>
-      <c r="M66" s="32"/>
-      <c r="N66" s="32"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="L66" s="35"/>
+      <c r="M66" s="35"/>
+      <c r="N66" s="35"/>
       <c r="O66" s="8"/>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="38"/>
-      <c r="S66" s="38"/>
-      <c r="T66" s="38"/>
+      <c r="P66" s="26"/>
+      <c r="Q66" s="26"/>
+      <c r="R66" s="26"/>
+      <c r="S66" s="26"/>
+      <c r="T66" s="26"/>
       <c r="U66" s="8"/>
-      <c r="V66" s="32"/>
-      <c r="W66" s="32"/>
-      <c r="X66" s="32"/>
+      <c r="V66" s="35"/>
+      <c r="W66" s="35"/>
+      <c r="X66" s="35"/>
       <c r="Y66" s="18"/>
       <c r="Z66" s="8"/>
       <c r="AA66" s="8" t="s">
@@ -5553,29 +5553,29 @@
       <c r="AK66" s="8"/>
     </row>
     <row r="67" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="32"/>
-      <c r="K67" s="32"/>
-      <c r="L67" s="32"/>
-      <c r="M67" s="32"/>
-      <c r="N67" s="32"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="35"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35"/>
       <c r="O67" s="8"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="38"/>
-      <c r="R67" s="38"/>
-      <c r="S67" s="38"/>
-      <c r="T67" s="38"/>
+      <c r="P67" s="26"/>
+      <c r="Q67" s="26"/>
+      <c r="R67" s="26"/>
+      <c r="S67" s="26"/>
+      <c r="T67" s="26"/>
       <c r="U67" s="8"/>
-      <c r="V67" s="32"/>
-      <c r="W67" s="32"/>
-      <c r="X67" s="32"/>
+      <c r="V67" s="35"/>
+      <c r="W67" s="35"/>
+      <c r="X67" s="35"/>
       <c r="Y67" s="18"/>
       <c r="Z67" s="8"/>
       <c r="AA67" s="8" t="s">
@@ -5635,31 +5635,31 @@
       <c r="AK68" s="8"/>
     </row>
     <row r="69" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="35" t="s">
+      <c r="G69" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="35"/>
-      <c r="L69" s="35"/>
-      <c r="M69" s="35"/>
-      <c r="N69" s="35"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="36"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+      <c r="N69" s="36"/>
       <c r="O69" s="8"/>
-      <c r="P69" s="35" t="s">
+      <c r="P69" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="Q69" s="35"/>
-      <c r="R69" s="35"/>
-      <c r="S69" s="35"/>
-      <c r="T69" s="35"/>
+      <c r="Q69" s="36"/>
+      <c r="R69" s="36"/>
+      <c r="S69" s="36"/>
+      <c r="T69" s="36"/>
       <c r="U69" s="8"/>
       <c r="V69" s="13"/>
       <c r="W69" s="13"/>
@@ -5681,31 +5681,31 @@
       <c r="AK69" s="8"/>
     </row>
     <row r="70" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="32" t="s">
+      <c r="G70" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H70" s="32"/>
-      <c r="I70" s="32"/>
-      <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
-      <c r="L70" s="32"/>
-      <c r="M70" s="32"/>
-      <c r="N70" s="32"/>
+      <c r="H70" s="35"/>
+      <c r="I70" s="35"/>
+      <c r="J70" s="35"/>
+      <c r="K70" s="35"/>
+      <c r="L70" s="35"/>
+      <c r="M70" s="35"/>
+      <c r="N70" s="35"/>
       <c r="O70" s="8"/>
-      <c r="P70" s="32" t="s">
+      <c r="P70" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="Q70" s="32"/>
-      <c r="R70" s="32"/>
-      <c r="S70" s="32"/>
-      <c r="T70" s="32"/>
+      <c r="Q70" s="35"/>
+      <c r="R70" s="35"/>
+      <c r="S70" s="35"/>
+      <c r="T70" s="35"/>
       <c r="U70" s="8"/>
       <c r="V70" s="13"/>
       <c r="W70" s="13"/>
@@ -5727,25 +5727,25 @@
       <c r="AK70" s="8"/>
     </row>
     <row r="71" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="32"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="32"/>
-      <c r="N71" s="32"/>
+      <c r="G71" s="35"/>
+      <c r="H71" s="35"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="35"/>
+      <c r="K71" s="35"/>
+      <c r="L71" s="35"/>
+      <c r="M71" s="35"/>
+      <c r="N71" s="35"/>
       <c r="O71" s="8"/>
-      <c r="P71" s="32"/>
-      <c r="Q71" s="32"/>
-      <c r="R71" s="32"/>
-      <c r="S71" s="32"/>
-      <c r="T71" s="32"/>
+      <c r="P71" s="35"/>
+      <c r="Q71" s="35"/>
+      <c r="R71" s="35"/>
+      <c r="S71" s="35"/>
+      <c r="T71" s="35"/>
       <c r="U71" s="8"/>
       <c r="V71" s="13"/>
       <c r="W71" s="13"/>
@@ -5767,25 +5767,25 @@
       <c r="AK71" s="8"/>
     </row>
     <row r="72" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
-      <c r="I72" s="32"/>
-      <c r="J72" s="32"/>
-      <c r="K72" s="32"/>
-      <c r="L72" s="32"/>
-      <c r="M72" s="32"/>
-      <c r="N72" s="32"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
+      <c r="L72" s="35"/>
+      <c r="M72" s="35"/>
+      <c r="N72" s="35"/>
       <c r="O72" s="8"/>
-      <c r="P72" s="32"/>
-      <c r="Q72" s="32"/>
-      <c r="R72" s="32"/>
-      <c r="S72" s="32"/>
-      <c r="T72" s="32"/>
+      <c r="P72" s="35"/>
+      <c r="Q72" s="35"/>
+      <c r="R72" s="35"/>
+      <c r="S72" s="35"/>
+      <c r="T72" s="35"/>
       <c r="U72" s="8"/>
       <c r="V72" s="13"/>
       <c r="W72" s="13"/>
@@ -5809,25 +5809,25 @@
       <c r="AK72" s="8"/>
     </row>
     <row r="73" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
       <c r="F73" s="8"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="32"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
-      <c r="N73" s="32"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="35"/>
+      <c r="K73" s="35"/>
+      <c r="L73" s="35"/>
+      <c r="M73" s="35"/>
+      <c r="N73" s="35"/>
       <c r="O73" s="8"/>
-      <c r="P73" s="32"/>
-      <c r="Q73" s="32"/>
-      <c r="R73" s="32"/>
-      <c r="S73" s="32"/>
-      <c r="T73" s="32"/>
+      <c r="P73" s="35"/>
+      <c r="Q73" s="35"/>
+      <c r="R73" s="35"/>
+      <c r="S73" s="35"/>
+      <c r="T73" s="35"/>
       <c r="U73" s="8"/>
       <c r="V73" s="8"/>
       <c r="W73" s="8"/>
@@ -5851,25 +5851,25 @@
       <c r="AK73" s="8"/>
     </row>
     <row r="74" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
       <c r="F74" s="8"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="32"/>
-      <c r="I74" s="32"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="35"/>
+      <c r="M74" s="35"/>
+      <c r="N74" s="35"/>
       <c r="O74" s="8"/>
-      <c r="P74" s="32"/>
-      <c r="Q74" s="32"/>
-      <c r="R74" s="32"/>
-      <c r="S74" s="32"/>
-      <c r="T74" s="32"/>
+      <c r="P74" s="35"/>
+      <c r="Q74" s="35"/>
+      <c r="R74" s="35"/>
+      <c r="S74" s="35"/>
+      <c r="T74" s="35"/>
       <c r="U74" s="8"/>
       <c r="V74" s="8"/>
       <c r="W74" s="8"/>
@@ -5893,25 +5893,25 @@
       <c r="AK74" s="8"/>
     </row>
     <row r="75" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
       <c r="F75" s="8"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="32"/>
-      <c r="I75" s="32"/>
-      <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
-      <c r="L75" s="32"/>
-      <c r="M75" s="32"/>
-      <c r="N75" s="32"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="35"/>
+      <c r="K75" s="35"/>
+      <c r="L75" s="35"/>
+      <c r="M75" s="35"/>
+      <c r="N75" s="35"/>
       <c r="O75" s="8"/>
-      <c r="P75" s="32"/>
-      <c r="Q75" s="32"/>
-      <c r="R75" s="32"/>
-      <c r="S75" s="32"/>
-      <c r="T75" s="32"/>
+      <c r="P75" s="35"/>
+      <c r="Q75" s="35"/>
+      <c r="R75" s="35"/>
+      <c r="S75" s="35"/>
+      <c r="T75" s="35"/>
       <c r="U75" s="8"/>
       <c r="V75" s="8"/>
       <c r="W75" s="8"/>
@@ -5935,25 +5935,25 @@
       <c r="AK75" s="8"/>
     </row>
     <row r="76" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
       <c r="F76" s="8"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="32"/>
-      <c r="I76" s="32"/>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-      <c r="M76" s="32"/>
-      <c r="N76" s="32"/>
+      <c r="G76" s="35"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="35"/>
+      <c r="J76" s="35"/>
+      <c r="K76" s="35"/>
+      <c r="L76" s="35"/>
+      <c r="M76" s="35"/>
+      <c r="N76" s="35"/>
       <c r="O76" s="8"/>
-      <c r="P76" s="32"/>
-      <c r="Q76" s="32"/>
-      <c r="R76" s="32"/>
-      <c r="S76" s="32"/>
-      <c r="T76" s="32"/>
+      <c r="P76" s="35"/>
+      <c r="Q76" s="35"/>
+      <c r="R76" s="35"/>
+      <c r="S76" s="35"/>
+      <c r="T76" s="35"/>
       <c r="U76" s="8"/>
       <c r="V76" s="8"/>
       <c r="W76" s="8"/>
@@ -5977,25 +5977,25 @@
       <c r="AK76" s="8"/>
     </row>
     <row r="77" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="32"/>
-      <c r="I77" s="32"/>
-      <c r="J77" s="32"/>
-      <c r="K77" s="32"/>
-      <c r="L77" s="32"/>
-      <c r="M77" s="32"/>
-      <c r="N77" s="32"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="35"/>
+      <c r="M77" s="35"/>
+      <c r="N77" s="35"/>
       <c r="O77" s="8"/>
-      <c r="P77" s="32"/>
-      <c r="Q77" s="32"/>
-      <c r="R77" s="32"/>
-      <c r="S77" s="32"/>
-      <c r="T77" s="32"/>
+      <c r="P77" s="35"/>
+      <c r="Q77" s="35"/>
+      <c r="R77" s="35"/>
+      <c r="S77" s="35"/>
+      <c r="T77" s="35"/>
       <c r="U77" s="8"/>
       <c r="V77" s="8"/>
       <c r="W77" s="8"/>
@@ -6019,25 +6019,25 @@
       <c r="AK77" s="8"/>
     </row>
     <row r="78" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
       <c r="F78" s="8"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="32"/>
-      <c r="I78" s="32"/>
-      <c r="J78" s="32"/>
-      <c r="K78" s="32"/>
-      <c r="L78" s="32"/>
-      <c r="M78" s="32"/>
-      <c r="N78" s="32"/>
+      <c r="G78" s="35"/>
+      <c r="H78" s="35"/>
+      <c r="I78" s="35"/>
+      <c r="J78" s="35"/>
+      <c r="K78" s="35"/>
+      <c r="L78" s="35"/>
+      <c r="M78" s="35"/>
+      <c r="N78" s="35"/>
       <c r="O78" s="8"/>
-      <c r="P78" s="32"/>
-      <c r="Q78" s="32"/>
-      <c r="R78" s="32"/>
-      <c r="S78" s="32"/>
-      <c r="T78" s="32"/>
+      <c r="P78" s="35"/>
+      <c r="Q78" s="35"/>
+      <c r="R78" s="35"/>
+      <c r="S78" s="35"/>
+      <c r="T78" s="35"/>
       <c r="U78" s="8"/>
       <c r="V78" s="8"/>
       <c r="W78" s="8"/>
@@ -6075,11 +6075,11 @@
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
       <c r="O79" s="8"/>
-      <c r="P79" s="32"/>
-      <c r="Q79" s="32"/>
-      <c r="R79" s="32"/>
-      <c r="S79" s="32"/>
-      <c r="T79" s="32"/>
+      <c r="P79" s="35"/>
+      <c r="Q79" s="35"/>
+      <c r="R79" s="35"/>
+      <c r="S79" s="35"/>
+      <c r="T79" s="35"/>
       <c r="U79" s="8"/>
       <c r="V79" s="8"/>
       <c r="W79" s="8"/>
@@ -6117,11 +6117,11 @@
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
       <c r="O80" s="8"/>
-      <c r="P80" s="32"/>
-      <c r="Q80" s="32"/>
-      <c r="R80" s="32"/>
-      <c r="S80" s="32"/>
-      <c r="T80" s="32"/>
+      <c r="P80" s="35"/>
+      <c r="Q80" s="35"/>
+      <c r="R80" s="35"/>
+      <c r="S80" s="35"/>
+      <c r="T80" s="35"/>
       <c r="U80" s="8"/>
       <c r="V80" s="8"/>
       <c r="W80" s="8"/>
@@ -6187,15 +6187,15 @@
       <c r="AK81" s="8"/>
     </row>
     <row r="82" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B82" s="39" t="s">
+      <c r="B82" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39" t="s">
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="F82" s="39"/>
+      <c r="F82" s="25"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
@@ -6233,11 +6233,11 @@
       <c r="AK82" s="8"/>
     </row>
     <row r="83" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
@@ -6278,16 +6278,16 @@
       <c r="B84" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="24" t="e">
+      <c r="C84" s="40" t="e">
         <f>AG19</f>
         <v>#N/A</v>
       </c>
-      <c r="D84" s="25"/>
-      <c r="E84" s="23" t="e">
+      <c r="D84" s="41"/>
+      <c r="E84" s="42" t="e">
         <f>_xlfn.RANK.EQ(C84,$C$84:$D$97)</f>
         <v>#N/A</v>
       </c>
-      <c r="F84" s="23"/>
+      <c r="F84" s="42"/>
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
@@ -6328,16 +6328,16 @@
       <c r="B85" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="24" t="e">
+      <c r="C85" s="40" t="e">
         <f t="shared" ref="C85:C98" si="2">AG20</f>
         <v>#N/A</v>
       </c>
-      <c r="D85" s="25"/>
-      <c r="E85" s="23" t="e">
+      <c r="D85" s="41"/>
+      <c r="E85" s="42" t="e">
         <f t="shared" ref="E85:E98" si="3">_xlfn.RANK.EQ(C85,$C$84:$D$97)</f>
         <v>#N/A</v>
       </c>
-      <c r="F85" s="23"/>
+      <c r="F85" s="42"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
@@ -6378,16 +6378,16 @@
       <c r="B86" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C86" s="24" t="e">
+      <c r="C86" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D86" s="25"/>
-      <c r="E86" s="23" t="e">
+      <c r="D86" s="41"/>
+      <c r="E86" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F86" s="23"/>
+      <c r="F86" s="42"/>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
@@ -6428,16 +6428,16 @@
       <c r="B87" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="24" t="e">
+      <c r="C87" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D87" s="25"/>
-      <c r="E87" s="23" t="e">
+      <c r="D87" s="41"/>
+      <c r="E87" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F87" s="23"/>
+      <c r="F87" s="42"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
@@ -6478,16 +6478,16 @@
       <c r="B88" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="24" t="e">
+      <c r="C88" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D88" s="25"/>
-      <c r="E88" s="23" t="e">
+      <c r="D88" s="41"/>
+      <c r="E88" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F88" s="23"/>
+      <c r="F88" s="42"/>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
@@ -6528,32 +6528,32 @@
       <c r="B89" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C89" s="24" t="e">
+      <c r="C89" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D89" s="25"/>
-      <c r="E89" s="23" t="e">
+      <c r="D89" s="41"/>
+      <c r="E89" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F89" s="23"/>
+      <c r="F89" s="42"/>
       <c r="G89" s="8"/>
-      <c r="H89" s="26" t="s">
+      <c r="H89" s="46" t="s">
         <v>260</v>
       </c>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
-      <c r="M89" s="27"/>
-      <c r="N89" s="27"/>
-      <c r="O89" s="27"/>
-      <c r="P89" s="27"/>
-      <c r="Q89" s="27"/>
-      <c r="R89" s="27"/>
-      <c r="S89" s="27"/>
-      <c r="T89" s="27"/>
+      <c r="I89" s="47"/>
+      <c r="J89" s="47"/>
+      <c r="K89" s="47"/>
+      <c r="L89" s="47"/>
+      <c r="M89" s="47"/>
+      <c r="N89" s="47"/>
+      <c r="O89" s="47"/>
+      <c r="P89" s="47"/>
+      <c r="Q89" s="47"/>
+      <c r="R89" s="47"/>
+      <c r="S89" s="47"/>
+      <c r="T89" s="47"/>
       <c r="U89" s="8"/>
       <c r="V89" s="8"/>
       <c r="W89" s="8"/>
@@ -6580,30 +6580,30 @@
       <c r="B90" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C90" s="24" t="e">
+      <c r="C90" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D90" s="25"/>
-      <c r="E90" s="23" t="e">
+      <c r="D90" s="41"/>
+      <c r="E90" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F90" s="23"/>
+      <c r="F90" s="42"/>
       <c r="G90" s="8"/>
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
-      <c r="M90" s="27"/>
-      <c r="N90" s="27"/>
-      <c r="O90" s="27"/>
-      <c r="P90" s="27"/>
-      <c r="Q90" s="27"/>
-      <c r="R90" s="27"/>
-      <c r="S90" s="27"/>
-      <c r="T90" s="27"/>
+      <c r="H90" s="47"/>
+      <c r="I90" s="47"/>
+      <c r="J90" s="47"/>
+      <c r="K90" s="47"/>
+      <c r="L90" s="47"/>
+      <c r="M90" s="47"/>
+      <c r="N90" s="47"/>
+      <c r="O90" s="47"/>
+      <c r="P90" s="47"/>
+      <c r="Q90" s="47"/>
+      <c r="R90" s="47"/>
+      <c r="S90" s="47"/>
+      <c r="T90" s="47"/>
       <c r="U90" s="8"/>
       <c r="V90" s="8"/>
       <c r="W90" s="8"/>
@@ -6630,30 +6630,30 @@
       <c r="B91" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C91" s="24" t="e">
+      <c r="C91" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D91" s="25"/>
-      <c r="E91" s="23" t="e">
+      <c r="D91" s="41"/>
+      <c r="E91" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F91" s="23"/>
+      <c r="F91" s="42"/>
       <c r="G91" s="8"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
-      <c r="M91" s="27"/>
-      <c r="N91" s="27"/>
-      <c r="O91" s="27"/>
-      <c r="P91" s="27"/>
-      <c r="Q91" s="27"/>
-      <c r="R91" s="27"/>
-      <c r="S91" s="27"/>
-      <c r="T91" s="27"/>
+      <c r="H91" s="47"/>
+      <c r="I91" s="47"/>
+      <c r="J91" s="47"/>
+      <c r="K91" s="47"/>
+      <c r="L91" s="47"/>
+      <c r="M91" s="47"/>
+      <c r="N91" s="47"/>
+      <c r="O91" s="47"/>
+      <c r="P91" s="47"/>
+      <c r="Q91" s="47"/>
+      <c r="R91" s="47"/>
+      <c r="S91" s="47"/>
+      <c r="T91" s="47"/>
       <c r="U91" s="8"/>
       <c r="V91" s="8"/>
       <c r="W91" s="8"/>
@@ -6680,30 +6680,30 @@
       <c r="B92" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="24" t="e">
+      <c r="C92" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D92" s="25"/>
-      <c r="E92" s="23" t="e">
+      <c r="D92" s="41"/>
+      <c r="E92" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F92" s="23"/>
+      <c r="F92" s="42"/>
       <c r="G92" s="8"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="N92" s="27"/>
-      <c r="O92" s="27"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="27"/>
-      <c r="R92" s="27"/>
-      <c r="S92" s="27"/>
-      <c r="T92" s="27"/>
+      <c r="H92" s="47"/>
+      <c r="I92" s="47"/>
+      <c r="J92" s="47"/>
+      <c r="K92" s="47"/>
+      <c r="L92" s="47"/>
+      <c r="M92" s="47"/>
+      <c r="N92" s="47"/>
+      <c r="O92" s="47"/>
+      <c r="P92" s="47"/>
+      <c r="Q92" s="47"/>
+      <c r="R92" s="47"/>
+      <c r="S92" s="47"/>
+      <c r="T92" s="47"/>
       <c r="U92" s="8"/>
       <c r="V92" s="8"/>
       <c r="W92" s="8"/>
@@ -6730,30 +6730,30 @@
       <c r="B93" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C93" s="24" t="e">
+      <c r="C93" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D93" s="25"/>
-      <c r="E93" s="23" t="e">
+      <c r="D93" s="41"/>
+      <c r="E93" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F93" s="23"/>
+      <c r="F93" s="42"/>
       <c r="G93" s="8"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="N93" s="27"/>
-      <c r="O93" s="27"/>
-      <c r="P93" s="27"/>
-      <c r="Q93" s="27"/>
-      <c r="R93" s="27"/>
-      <c r="S93" s="27"/>
-      <c r="T93" s="27"/>
+      <c r="H93" s="47"/>
+      <c r="I93" s="47"/>
+      <c r="J93" s="47"/>
+      <c r="K93" s="47"/>
+      <c r="L93" s="47"/>
+      <c r="M93" s="47"/>
+      <c r="N93" s="47"/>
+      <c r="O93" s="47"/>
+      <c r="P93" s="47"/>
+      <c r="Q93" s="47"/>
+      <c r="R93" s="47"/>
+      <c r="S93" s="47"/>
+      <c r="T93" s="47"/>
       <c r="U93" s="8"/>
       <c r="V93" s="8"/>
       <c r="W93" s="8"/>
@@ -6780,30 +6780,30 @@
       <c r="B94" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C94" s="24" t="e">
+      <c r="C94" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D94" s="25"/>
-      <c r="E94" s="23" t="e">
+      <c r="D94" s="41"/>
+      <c r="E94" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F94" s="23"/>
+      <c r="F94" s="42"/>
       <c r="G94" s="8"/>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
-      <c r="M94" s="27"/>
-      <c r="N94" s="27"/>
-      <c r="O94" s="27"/>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="27"/>
-      <c r="R94" s="27"/>
-      <c r="S94" s="27"/>
-      <c r="T94" s="27"/>
+      <c r="H94" s="47"/>
+      <c r="I94" s="47"/>
+      <c r="J94" s="47"/>
+      <c r="K94" s="47"/>
+      <c r="L94" s="47"/>
+      <c r="M94" s="47"/>
+      <c r="N94" s="47"/>
+      <c r="O94" s="47"/>
+      <c r="P94" s="47"/>
+      <c r="Q94" s="47"/>
+      <c r="R94" s="47"/>
+      <c r="S94" s="47"/>
+      <c r="T94" s="47"/>
       <c r="U94" s="8"/>
       <c r="V94" s="8"/>
       <c r="W94" s="8"/>
@@ -6830,30 +6830,30 @@
       <c r="B95" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C95" s="24" t="e">
+      <c r="C95" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D95" s="25"/>
-      <c r="E95" s="23" t="e">
+      <c r="D95" s="41"/>
+      <c r="E95" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F95" s="23"/>
+      <c r="F95" s="42"/>
       <c r="G95" s="8"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
-      <c r="M95" s="27"/>
-      <c r="N95" s="27"/>
-      <c r="O95" s="27"/>
-      <c r="P95" s="27"/>
-      <c r="Q95" s="27"/>
-      <c r="R95" s="27"/>
-      <c r="S95" s="27"/>
-      <c r="T95" s="27"/>
+      <c r="H95" s="47"/>
+      <c r="I95" s="47"/>
+      <c r="J95" s="47"/>
+      <c r="K95" s="47"/>
+      <c r="L95" s="47"/>
+      <c r="M95" s="47"/>
+      <c r="N95" s="47"/>
+      <c r="O95" s="47"/>
+      <c r="P95" s="47"/>
+      <c r="Q95" s="47"/>
+      <c r="R95" s="47"/>
+      <c r="S95" s="47"/>
+      <c r="T95" s="47"/>
       <c r="U95" s="8"/>
       <c r="V95" s="8"/>
       <c r="W95" s="8"/>
@@ -6880,16 +6880,16 @@
       <c r="B96" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C96" s="24" t="e">
+      <c r="C96" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D96" s="25"/>
-      <c r="E96" s="23" t="e">
+      <c r="D96" s="41"/>
+      <c r="E96" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="23"/>
+      <c r="F96" s="42"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
@@ -6930,16 +6930,16 @@
       <c r="B97" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C97" s="24" t="e">
+      <c r="C97" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D97" s="25"/>
-      <c r="E97" s="23" t="e">
+      <c r="D97" s="41"/>
+      <c r="E97" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F97" s="23"/>
+      <c r="F97" s="42"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
       <c r="I97" s="8"/>
@@ -6980,32 +6980,32 @@
       <c r="B98" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C98" s="24" t="e">
+      <c r="C98" s="40" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="D98" s="25"/>
-      <c r="E98" s="23" t="e">
+      <c r="D98" s="41"/>
+      <c r="E98" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="F98" s="23"/>
+      <c r="F98" s="42"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
-      <c r="I98" s="28" t="s">
+      <c r="I98" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="J98" s="29"/>
-      <c r="K98" s="29"/>
-      <c r="L98" s="29"/>
-      <c r="M98" s="29"/>
-      <c r="N98" s="29"/>
-      <c r="O98" s="29"/>
-      <c r="P98" s="29"/>
-      <c r="Q98" s="29"/>
-      <c r="R98" s="29"/>
-      <c r="S98" s="29"/>
-      <c r="T98" s="29"/>
+      <c r="J98" s="49"/>
+      <c r="K98" s="49"/>
+      <c r="L98" s="49"/>
+      <c r="M98" s="49"/>
+      <c r="N98" s="49"/>
+      <c r="O98" s="49"/>
+      <c r="P98" s="49"/>
+      <c r="Q98" s="49"/>
+      <c r="R98" s="49"/>
+      <c r="S98" s="49"/>
+      <c r="T98" s="49"/>
       <c r="U98" s="8"/>
       <c r="V98" s="8"/>
       <c r="W98" s="8"/>
@@ -7036,18 +7036,18 @@
       <c r="F99" s="8"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
-      <c r="I99" s="29"/>
-      <c r="J99" s="29"/>
-      <c r="K99" s="29"/>
-      <c r="L99" s="29"/>
-      <c r="M99" s="29"/>
-      <c r="N99" s="29"/>
-      <c r="O99" s="29"/>
-      <c r="P99" s="29"/>
-      <c r="Q99" s="29"/>
-      <c r="R99" s="29"/>
-      <c r="S99" s="29"/>
-      <c r="T99" s="29"/>
+      <c r="I99" s="49"/>
+      <c r="J99" s="49"/>
+      <c r="K99" s="49"/>
+      <c r="L99" s="49"/>
+      <c r="M99" s="49"/>
+      <c r="N99" s="49"/>
+      <c r="O99" s="49"/>
+      <c r="P99" s="49"/>
+      <c r="Q99" s="49"/>
+      <c r="R99" s="49"/>
+      <c r="S99" s="49"/>
+      <c r="T99" s="49"/>
       <c r="U99" s="8"/>
       <c r="V99" s="8"/>
       <c r="W99" s="8"/>
@@ -7078,18 +7078,18 @@
       <c r="F100" s="8"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
-      <c r="I100" s="29"/>
-      <c r="J100" s="29"/>
-      <c r="K100" s="29"/>
-      <c r="L100" s="29"/>
-      <c r="M100" s="29"/>
-      <c r="N100" s="29"/>
-      <c r="O100" s="29"/>
-      <c r="P100" s="29"/>
-      <c r="Q100" s="29"/>
-      <c r="R100" s="29"/>
-      <c r="S100" s="29"/>
-      <c r="T100" s="29"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="49"/>
+      <c r="K100" s="49"/>
+      <c r="L100" s="49"/>
+      <c r="M100" s="49"/>
+      <c r="N100" s="49"/>
+      <c r="O100" s="49"/>
+      <c r="P100" s="49"/>
+      <c r="Q100" s="49"/>
+      <c r="R100" s="49"/>
+      <c r="S100" s="49"/>
+      <c r="T100" s="49"/>
       <c r="U100" s="8"/>
       <c r="V100" s="8"/>
       <c r="W100" s="8"/>
@@ -7120,18 +7120,18 @@
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
       <c r="H101" s="8"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-      <c r="K101" s="29"/>
-      <c r="L101" s="29"/>
-      <c r="M101" s="29"/>
-      <c r="N101" s="29"/>
-      <c r="O101" s="29"/>
-      <c r="P101" s="29"/>
-      <c r="Q101" s="29"/>
-      <c r="R101" s="29"/>
-      <c r="S101" s="29"/>
-      <c r="T101" s="29"/>
+      <c r="I101" s="49"/>
+      <c r="J101" s="49"/>
+      <c r="K101" s="49"/>
+      <c r="L101" s="49"/>
+      <c r="M101" s="49"/>
+      <c r="N101" s="49"/>
+      <c r="O101" s="49"/>
+      <c r="P101" s="49"/>
+      <c r="Q101" s="49"/>
+      <c r="R101" s="49"/>
+      <c r="S101" s="49"/>
+      <c r="T101" s="49"/>
       <c r="U101" s="8"/>
       <c r="V101" s="8"/>
       <c r="W101" s="8"/>
@@ -7163,19 +7163,19 @@
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
-      <c r="J102" s="30" t="s">
+      <c r="J102" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="K102" s="31"/>
-      <c r="L102" s="31"/>
-      <c r="M102" s="31"/>
-      <c r="N102" s="31"/>
-      <c r="O102" s="31"/>
-      <c r="P102" s="31"/>
-      <c r="Q102" s="31"/>
-      <c r="R102" s="31"/>
-      <c r="S102" s="31"/>
-      <c r="T102" s="31"/>
+      <c r="K102" s="51"/>
+      <c r="L102" s="51"/>
+      <c r="M102" s="51"/>
+      <c r="N102" s="51"/>
+      <c r="O102" s="51"/>
+      <c r="P102" s="51"/>
+      <c r="Q102" s="51"/>
+      <c r="R102" s="51"/>
+      <c r="S102" s="51"/>
+      <c r="T102" s="51"/>
       <c r="U102" s="8"/>
       <c r="V102" s="8"/>
       <c r="W102" s="8"/>
@@ -7207,17 +7207,17 @@
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
-      <c r="J103" s="31"/>
-      <c r="K103" s="31"/>
-      <c r="L103" s="31"/>
-      <c r="M103" s="31"/>
-      <c r="N103" s="31"/>
-      <c r="O103" s="31"/>
-      <c r="P103" s="31"/>
-      <c r="Q103" s="31"/>
-      <c r="R103" s="31"/>
-      <c r="S103" s="31"/>
-      <c r="T103" s="31"/>
+      <c r="J103" s="51"/>
+      <c r="K103" s="51"/>
+      <c r="L103" s="51"/>
+      <c r="M103" s="51"/>
+      <c r="N103" s="51"/>
+      <c r="O103" s="51"/>
+      <c r="P103" s="51"/>
+      <c r="Q103" s="51"/>
+      <c r="R103" s="51"/>
+      <c r="S103" s="51"/>
+      <c r="T103" s="51"/>
       <c r="U103" s="8"/>
       <c r="V103" s="8"/>
       <c r="W103" s="8"/>
@@ -7249,17 +7249,17 @@
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
-      <c r="J104" s="31"/>
-      <c r="K104" s="31"/>
-      <c r="L104" s="31"/>
-      <c r="M104" s="31"/>
-      <c r="N104" s="31"/>
-      <c r="O104" s="31"/>
-      <c r="P104" s="31"/>
-      <c r="Q104" s="31"/>
-      <c r="R104" s="31"/>
-      <c r="S104" s="31"/>
-      <c r="T104" s="31"/>
+      <c r="J104" s="51"/>
+      <c r="K104" s="51"/>
+      <c r="L104" s="51"/>
+      <c r="M104" s="51"/>
+      <c r="N104" s="51"/>
+      <c r="O104" s="51"/>
+      <c r="P104" s="51"/>
+      <c r="Q104" s="51"/>
+      <c r="R104" s="51"/>
+      <c r="S104" s="51"/>
+      <c r="T104" s="51"/>
       <c r="U104" s="8"/>
       <c r="V104" s="8"/>
       <c r="W104" s="8"/>
@@ -8023,6 +8023,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="H89:T95"/>
+    <mergeCell ref="I98:T101"/>
+    <mergeCell ref="J102:T104"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="B43:E54"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="G43:N54"/>
+    <mergeCell ref="G42:N42"/>
+    <mergeCell ref="G56:N56"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="P56:T56"/>
+    <mergeCell ref="V57:X67"/>
+    <mergeCell ref="V56:X56"/>
+    <mergeCell ref="V42:X42"/>
+    <mergeCell ref="V43:X51"/>
+    <mergeCell ref="Q42:T42"/>
+    <mergeCell ref="Q43:T52"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B57:E67"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="G69:N69"/>
+    <mergeCell ref="P69:T69"/>
+    <mergeCell ref="B70:E78"/>
+    <mergeCell ref="G70:N78"/>
+    <mergeCell ref="P57:T67"/>
+    <mergeCell ref="G57:N67"/>
+    <mergeCell ref="P70:T80"/>
+    <mergeCell ref="B82:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E82:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="Q40:T40"/>
+    <mergeCell ref="V39:X39"/>
+    <mergeCell ref="V40:X40"/>
+    <mergeCell ref="Q39:T39"/>
+    <mergeCell ref="B34:T35"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="G40:N40"/>
+    <mergeCell ref="G39:N39"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="S26:W28"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="T18:W18"/>
@@ -8039,72 +8105,6 @@
     <mergeCell ref="B13:X14"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="P16:R16"/>
-    <mergeCell ref="Q40:T40"/>
-    <mergeCell ref="V39:X39"/>
-    <mergeCell ref="V40:X40"/>
-    <mergeCell ref="Q39:T39"/>
-    <mergeCell ref="B34:T35"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="G40:N40"/>
-    <mergeCell ref="G39:N39"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="B57:E67"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="G69:N69"/>
-    <mergeCell ref="P69:T69"/>
-    <mergeCell ref="B70:E78"/>
-    <mergeCell ref="G70:N78"/>
-    <mergeCell ref="P57:T67"/>
-    <mergeCell ref="G57:N67"/>
-    <mergeCell ref="P70:T80"/>
-    <mergeCell ref="B82:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E82:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="P56:T56"/>
-    <mergeCell ref="V57:X67"/>
-    <mergeCell ref="V56:X56"/>
-    <mergeCell ref="V42:X42"/>
-    <mergeCell ref="V43:X51"/>
-    <mergeCell ref="Q42:T42"/>
-    <mergeCell ref="Q43:T52"/>
-    <mergeCell ref="B43:E54"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="G43:N54"/>
-    <mergeCell ref="G42:N42"/>
-    <mergeCell ref="G56:N56"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="H89:T95"/>
-    <mergeCell ref="I98:T101"/>
-    <mergeCell ref="J102:T104"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
   </mergeCells>
   <conditionalFormatting sqref="C84:D98">
     <cfRule type="colorScale" priority="1">
@@ -8546,7 +8546,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8579,7 +8579,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>2</v>
@@ -8834,16 +8834,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF98156A4E08ED42B22DA6C86624442E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11ba5f1833b47c39d11f9a0fc9ca5ad0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56528f00-8daf-4285-8b2f-184ebce7f2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b814f87d70368c36b985d9f62a71433" ns2:_="">
     <xsd:import namespace="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
@@ -9021,6 +9011,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56528f00-8daf-4285-8b2f-184ebce7f2e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9031,22 +9031,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{868C143E-6D51-4467-8AC0-C13BFF0C5CF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00089E46-9D1D-406D-80DB-769E94388862}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9065,6 +9049,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{868C143E-6D51-4467-8AC0-C13BFF0C5CF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56528f00-8daf-4285-8b2f-184ebce7f2e9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E55394AD-EAD7-4DB0-8A63-1FFADDFE8C2B}">
   <ds:schemaRefs>

</xml_diff>